<commit_message>
validación de superviso pgt
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaCnpc - copia.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaCnpc - copia.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6EC891-F62D-4794-BE28-D49FADEA597E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D48D791-460B-4996-952A-22C06003A326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{A8A21D80-6B9E-470C-B871-94B7E315DE21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A8A21D80-6B9E-470C-B871-94B7E315DE21}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cantidad&amp;Calidad_CNPC" sheetId="1" r:id="rId1"/>
-    <sheet name="Boleta_CNPC" sheetId="2" r:id="rId2"/>
+    <sheet name="Boleta_CNPC" sheetId="2" r:id="rId1"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
@@ -26,81 +26,43 @@
     <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
-    <externalReference r:id="rId12"/>
-    <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_01_Dic_00" localSheetId="0">#REF!</definedName>
     <definedName name="_01_Dic_00">#REF!</definedName>
-    <definedName name="_01_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_01_Mar_98">#REF!</definedName>
-    <definedName name="_01_Oct_99" localSheetId="0">#REF!</definedName>
     <definedName name="_01_Oct_99">#REF!</definedName>
-    <definedName name="_02_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_02_Mar_98">#REF!</definedName>
-    <definedName name="_03_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_03_Mar_98">#REF!</definedName>
-    <definedName name="_04_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_04_Mar_98">#REF!</definedName>
-    <definedName name="_05_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_05_Mar_98">#REF!</definedName>
-    <definedName name="_06_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_06_Mar_98">#REF!</definedName>
-    <definedName name="_07_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_07_Mar_98">#REF!</definedName>
-    <definedName name="_08_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_08_Mar_98">#REF!</definedName>
-    <definedName name="_09_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_09_Mar_98">#REF!</definedName>
-    <definedName name="_1_Jul_99" localSheetId="0">#REF!</definedName>
     <definedName name="_1_Jul_99">#REF!</definedName>
-    <definedName name="_10_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_10_Mar_98">#REF!</definedName>
-    <definedName name="_11_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_11_Mar_98">#REF!</definedName>
-    <definedName name="_12_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_12_Mar_98">#REF!</definedName>
-    <definedName name="_13_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_13_Mar_98">#REF!</definedName>
-    <definedName name="_14_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_14_Mar_98">#REF!</definedName>
-    <definedName name="_15_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_15_Mar_98">#REF!</definedName>
-    <definedName name="_16_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_16_Mar_98">#REF!</definedName>
-    <definedName name="_17_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_17_Mar_98">#REF!</definedName>
-    <definedName name="_18_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_18_Mar_98">#REF!</definedName>
-    <definedName name="_19_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_19_Mar_98">#REF!</definedName>
-    <definedName name="_20_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_20_Mar_98">#REF!</definedName>
-    <definedName name="_21_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_21_Mar_98">#REF!</definedName>
-    <definedName name="_22_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_22_Mar_98">#REF!</definedName>
-    <definedName name="_23_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_23_Mar_98">#REF!</definedName>
-    <definedName name="_24_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_24_Mar_98">#REF!</definedName>
-    <definedName name="_25_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_25_Mar_98">#REF!</definedName>
-    <definedName name="_26_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_26_Mar_98">#REF!</definedName>
-    <definedName name="_27_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_27_Mar_98">#REF!</definedName>
-    <definedName name="_28_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_28_Mar_98">#REF!</definedName>
-    <definedName name="_29_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_29_Mar_98">#REF!</definedName>
-    <definedName name="_30_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_30_Mar_98">#REF!</definedName>
-    <definedName name="_31_Jul_99" localSheetId="0">#REF!</definedName>
     <definedName name="_31_Jul_99">#REF!</definedName>
-    <definedName name="_31_Mar_98" localSheetId="0">#REF!</definedName>
     <definedName name="_31_Mar_98">#REF!</definedName>
-    <definedName name="_Ago07" localSheetId="0">'[1]balance diario'!#REF!</definedName>
     <definedName name="_Ago07">'[1]balance diario'!#REF!</definedName>
     <definedName name="_OCT10">[2]ROMT!$BE$439:$BL$442</definedName>
     <definedName name="_OCT11">[2]ROMT!$BE$487:$BL$490</definedName>
@@ -108,9 +70,7 @@
     <definedName name="_OCT13">[2]ROMT!$BE$587:$BL$590</definedName>
     <definedName name="_OCT14">[2]ROMT!$BE$637:$BL$640</definedName>
     <definedName name="_OCT2">[2]ROMT!$BE$82:$BL$85</definedName>
-    <definedName name="_OCT20" localSheetId="0">#REF!</definedName>
     <definedName name="_OCT20">#REF!</definedName>
-    <definedName name="_OCT21" localSheetId="0">#REF!</definedName>
     <definedName name="_OCT21">#REF!</definedName>
     <definedName name="_OCT3">[2]ROMT!$BE$143:$BL$147</definedName>
     <definedName name="_OCT4">[2]ROMT!$BE$191:$BL$195</definedName>
@@ -118,14 +78,10 @@
     <definedName name="_OCT6">[2]ROMT!$BE$291:$BL$294</definedName>
     <definedName name="_OCT7">[2]ROMT!$BE$338:$BL$342</definedName>
     <definedName name="_OCT9">[2]ROMT!$BE$389:$BL$392</definedName>
-    <definedName name="_PPP500" localSheetId="0">#REF!</definedName>
     <definedName name="_PPP500">#REF!</definedName>
-    <definedName name="_R" localSheetId="0">#REF!</definedName>
     <definedName name="_R">#REF!</definedName>
-    <definedName name="_TAQ1" localSheetId="0">#REF!</definedName>
     <definedName name="_TAQ1">#REF!</definedName>
     <definedName name="_TAQ5">[3]TABLAS!$BE$200:$BQ$234</definedName>
-    <definedName name="_TEX500" localSheetId="0">#REF!</definedName>
     <definedName name="_TEX500">#REF!</definedName>
     <definedName name="_TQ1">[2]ROMT!$BE$1:$BQ$37</definedName>
     <definedName name="_TQ10">[2]ROMT!$BE$400:$BQ$437</definedName>
@@ -133,177 +89,115 @@
     <definedName name="_TQ12">[2]ROMT!$BE$500:$BQ$535</definedName>
     <definedName name="_TQ13">[2]ROMT!$BE$550:$BQ$585</definedName>
     <definedName name="_TQ14">[2]ROMT!$BE$600:$BQ$635</definedName>
-    <definedName name="_TQ18" localSheetId="0">#REF!</definedName>
     <definedName name="_TQ18">#REF!</definedName>
     <definedName name="_TQ2">[2]ROMT!$BE$50:$BQ$80</definedName>
-    <definedName name="_TQ20" localSheetId="0">#REF!</definedName>
     <definedName name="_TQ20">#REF!</definedName>
-    <definedName name="_TQ21" localSheetId="0">#REF!</definedName>
     <definedName name="_TQ21">#REF!</definedName>
     <definedName name="_TQ3">[2]ROMT!$BE$100:$BQ$141</definedName>
     <definedName name="_TQ4">[2]ROMT!$BE$150:$BQ$189</definedName>
     <definedName name="_TQ5">[2]ROMT!$BE$200:$BQ$234</definedName>
-    <definedName name="_TQ50" localSheetId="0">#REF!</definedName>
     <definedName name="_TQ50">#REF!</definedName>
     <definedName name="_TQ6">[2]ROMT!$BE$250:$BQ$289</definedName>
     <definedName name="_TQ7">[2]ROMT!$BE$300:$BQ$336</definedName>
     <definedName name="_TQ9">[2]ROMT!$BE$350:$BQ$387</definedName>
-    <definedName name="_TT14" localSheetId="0">#REF!</definedName>
     <definedName name="_TT14">#REF!</definedName>
-    <definedName name="_TT21" localSheetId="0">#REF!</definedName>
     <definedName name="_TT21">#REF!</definedName>
-    <definedName name="_TTA1" localSheetId="0">#REF!</definedName>
     <definedName name="_TTA1">#REF!</definedName>
-    <definedName name="_TTD2" localSheetId="0">#REF!</definedName>
     <definedName name="_TTD2">#REF!</definedName>
-    <definedName name="AAA" localSheetId="0">#REF!</definedName>
     <definedName name="AAA">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Boleta_CNPC!$B$1:$J$64</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Cantidad&amp;Calidad_CNPC'!$A$1:$S$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Boleta_CNPC!$B$1:$J$60</definedName>
     <definedName name="_xlnm.Database">'[4]TABLA TRINITY'!#REF!</definedName>
-    <definedName name="BBB" localSheetId="0">#REF!</definedName>
     <definedName name="BBB">#REF!</definedName>
-    <definedName name="CCC" localSheetId="0">#REF!</definedName>
     <definedName name="CCC">#REF!</definedName>
     <definedName name="CO">[5]corcerviz!$A$8:$T$38</definedName>
-    <definedName name="CONCERDIESEL" localSheetId="0">#REF!</definedName>
     <definedName name="CONCERDIESEL">#REF!</definedName>
-    <definedName name="CORD2" localSheetId="0">#REF!</definedName>
     <definedName name="CORD2">#REF!</definedName>
-    <definedName name="DDD" localSheetId="0">#REF!</definedName>
     <definedName name="DDD">#REF!</definedName>
-    <definedName name="DDDD" localSheetId="0">#REF!</definedName>
     <definedName name="DDDD">#REF!</definedName>
-    <definedName name="DESPACHO" localSheetId="0">#REF!</definedName>
     <definedName name="DESPACHO">#REF!</definedName>
-    <definedName name="DIARIO" localSheetId="0">#REF!</definedName>
     <definedName name="DIARIO">#REF!</definedName>
+    <definedName name="FactoresDistribucionGasCombustible_item">Boleta_CNPC!#REF!</definedName>
+    <definedName name="FactoresDistribucionGasCombustible_itemd">Boleta_CNPC!#REF!</definedName>
+    <definedName name="FactoresDistribucionGasCombustible_Items">Boleta_CNPC!#REF!</definedName>
+    <definedName name="FactoresDistribucionGasCombustible_itemss">Boleta_CNPC!#REF!</definedName>
+    <definedName name="FactoresDistribucionGasDeCombustible_item">Boleta_CNPC!$B$35:$I$36</definedName>
+    <definedName name="FactoresDistribucionGasDeCombustible_Items">Boleta_CNPC!$B$35:$I$36</definedName>
     <definedName name="FactoresDistribucionGasNaturalSeco_item">Boleta_CNPC!$B$19:$I$20</definedName>
     <definedName name="FactoresDistribucionGasNaturalSeco_Items">Boleta_CNPC!$B$19:$I$20</definedName>
+    <definedName name="FactoresDistribucionLiquidoGasNatural_item">Boleta_CNPC!#REF!</definedName>
+    <definedName name="FactoresDistribucionLiquidoGasNatural_Items">Boleta_CNPC!$B$51:$I$52</definedName>
     <definedName name="Firmas">INDEX('[6]DATOS CORREOS'!$L$2:$L$9,MATCH([6]Datos!$U$2,'[6]DATOS CORREOS'!$K$2:$K$9,0))</definedName>
-    <definedName name="GGG" localSheetId="0">#REF!</definedName>
     <definedName name="GGG">#REF!</definedName>
-    <definedName name="HORARIO" localSheetId="0">#REF!</definedName>
     <definedName name="HORARIO">#REF!</definedName>
-    <definedName name="HORAS" localSheetId="0">#REF!</definedName>
     <definedName name="HORAS">#REF!</definedName>
-    <definedName name="INVROMT" localSheetId="0">#REF!</definedName>
     <definedName name="INVROMT">#REF!</definedName>
-    <definedName name="MAR" localSheetId="0">#REF!</definedName>
+    <definedName name="Item.Sumistrador">Boleta_CNPC!#REF!</definedName>
+    <definedName name="Items.Sumistrador">Boleta_CNPC!#REF!</definedName>
     <definedName name="MAR">#REF!</definedName>
-    <definedName name="MARCIANITO" localSheetId="0">#REF!</definedName>
     <definedName name="MARCIANITO">#REF!</definedName>
-    <definedName name="MARCIANITO20" localSheetId="0">#REF!</definedName>
     <definedName name="MARCIANITO20">#REF!</definedName>
-    <definedName name="MARCIANITO21" localSheetId="0">#REF!</definedName>
     <definedName name="MARCIANITO21">#REF!</definedName>
-    <definedName name="MARCON" localSheetId="0">#REF!</definedName>
     <definedName name="MARCON">#REF!</definedName>
     <definedName name="MESTEMP">'[7]DATOS 2'!$BG$6:$BL$17</definedName>
     <definedName name="MO">[5]mobil!$A$8:$T$38</definedName>
-    <definedName name="MOBILD2" localSheetId="0">#REF!</definedName>
     <definedName name="MOBILD2">#REF!</definedName>
-    <definedName name="MPGGAS90" localSheetId="0">#REF!</definedName>
     <definedName name="MPGGAS90">#REF!</definedName>
     <definedName name="Nov">'[1]balance diario'!#REF!</definedName>
     <definedName name="OCTV5">[3]TABLAS!$BE$236:$BL$239</definedName>
-    <definedName name="OLE_LINK4" localSheetId="0">'[8]7_Mensaje'!#REF!</definedName>
     <definedName name="OLE_LINK4">'[6]7_Mensaje'!#REF!</definedName>
-    <definedName name="OTROS" localSheetId="0">#REF!</definedName>
     <definedName name="OTROS">#REF!</definedName>
     <definedName name="PE">[5]pecsa!$A$8:$T$38</definedName>
-    <definedName name="PECSAD2" localSheetId="0">#REF!</definedName>
     <definedName name="PECSAD2">#REF!</definedName>
-    <definedName name="PECSAGAS84" localSheetId="0">#REF!</definedName>
     <definedName name="PECSAGAS84">#REF!</definedName>
-    <definedName name="PECSAHORA" localSheetId="0">#REF!</definedName>
     <definedName name="PECSAHORA">#REF!</definedName>
-    <definedName name="PECSAKERO" localSheetId="0">#REF!</definedName>
     <definedName name="PECSAKERO">#REF!</definedName>
-    <definedName name="PEREZ">'[9]COMPRAS DE GAS'!$H$1:$M$51</definedName>
-    <definedName name="PET" localSheetId="0">#REF!</definedName>
+    <definedName name="PEREZ">'[8]COMPRAS DE GAS'!$H$1:$M$51</definedName>
     <definedName name="PET">#REF!</definedName>
-    <definedName name="PETORTECH">'[9]COMPRAS DE GAS'!$A$1:$F$51</definedName>
-    <definedName name="POZA" localSheetId="0">#REF!</definedName>
+    <definedName name="PETORTECH">'[8]COMPRAS DE GAS'!$A$1:$F$51</definedName>
     <definedName name="POZA">#REF!</definedName>
     <definedName name="PP">[5]petroperu!$A$8:$T$38</definedName>
-    <definedName name="PPDIESEL" localSheetId="0">#REF!</definedName>
     <definedName name="PPDIESEL">#REF!</definedName>
-    <definedName name="PPGAS84" localSheetId="0">#REF!</definedName>
     <definedName name="PPGAS84">#REF!</definedName>
-    <definedName name="PPGAS90" localSheetId="0">#REF!</definedName>
     <definedName name="PPGAS90">#REF!</definedName>
-    <definedName name="PPKERO" localSheetId="0">#REF!</definedName>
     <definedName name="PPKERO">#REF!</definedName>
-    <definedName name="PPRC250" localSheetId="0">#REF!</definedName>
     <definedName name="PPRC250">#REF!</definedName>
-    <definedName name="PPTURBO" localSheetId="0">#REF!</definedName>
     <definedName name="PPTURBO">#REF!</definedName>
     <definedName name="RE">[5]relapasa!$A$8:$T$38</definedName>
-    <definedName name="REFDIESEL" localSheetId="0">#REF!</definedName>
     <definedName name="REFDIESEL">#REF!</definedName>
-    <definedName name="REFGAS84" localSheetId="0">#REF!</definedName>
     <definedName name="REFGAS84">#REF!</definedName>
-    <definedName name="REFGAS90" localSheetId="0">#REF!</definedName>
     <definedName name="REFGAS90">#REF!</definedName>
-    <definedName name="REFKERO" localSheetId="0">#REF!</definedName>
     <definedName name="REFKERO">#REF!</definedName>
-    <definedName name="REFP500" localSheetId="0">#REF!</definedName>
     <definedName name="REFP500">#REF!</definedName>
-    <definedName name="REFPI5000" localSheetId="0">#REF!</definedName>
     <definedName name="REFPI5000">#REF!</definedName>
-    <definedName name="REFRC250" localSheetId="0">#REF!</definedName>
     <definedName name="REFRC250">#REF!</definedName>
-    <definedName name="REFTURBO" localSheetId="0">#REF!</definedName>
     <definedName name="REFTURBO">#REF!</definedName>
-    <definedName name="REL" localSheetId="0">#REF!</definedName>
     <definedName name="REL">#REF!</definedName>
-    <definedName name="RELAPITA" localSheetId="0">#REF!</definedName>
     <definedName name="RELAPITA">#REF!</definedName>
-    <definedName name="reporte" localSheetId="0">#REF!</definedName>
     <definedName name="reporte">#REF!</definedName>
-    <definedName name="REPORTE_DIARIO" localSheetId="0">#REF!</definedName>
     <definedName name="REPORTE_DIARIO">#REF!</definedName>
-    <definedName name="REPORTE1" localSheetId="0">#REF!</definedName>
     <definedName name="REPORTE1">#REF!</definedName>
-    <definedName name="SDIESEL" localSheetId="0">#REF!</definedName>
     <definedName name="SDIESEL">#REF!</definedName>
-    <definedName name="SGAS84">'[10]#¡REF'!$U$47:$AE$77</definedName>
-    <definedName name="SGAS90" localSheetId="0">#REF!</definedName>
+    <definedName name="SGAS84">'[9]#¡REF'!$U$47:$AE$77</definedName>
     <definedName name="SGAS90">#REF!</definedName>
     <definedName name="SH">[5]shell!$A$8:$T$38</definedName>
-    <definedName name="SHELLD2" localSheetId="0">#REF!</definedName>
     <definedName name="SHELLD2">#REF!</definedName>
-    <definedName name="SHELLGAS90" localSheetId="0">#REF!</definedName>
     <definedName name="SHELLGAS90">#REF!</definedName>
-    <definedName name="SHELLPI500" localSheetId="0">#REF!</definedName>
     <definedName name="SHELLPI500">#REF!</definedName>
-    <definedName name="SKERO" localSheetId="0">#REF!</definedName>
     <definedName name="SKERO">#REF!</definedName>
-    <definedName name="TANQUE2" localSheetId="0">#REF!</definedName>
     <definedName name="TANQUE2">#REF!</definedName>
     <definedName name="TE">[5]texaco!$A$8:$T$38</definedName>
-    <definedName name="TEXCIESEL" localSheetId="0">#REF!</definedName>
     <definedName name="TEXCIESEL">#REF!</definedName>
-    <definedName name="TEXDIESEL" localSheetId="0">#REF!</definedName>
     <definedName name="TEXDIESEL">#REF!</definedName>
-    <definedName name="TEXKERO" localSheetId="0">#REF!</definedName>
     <definedName name="TEXKERO">#REF!</definedName>
-    <definedName name="TK_4601">'[11]REPORTE hoja2 (12h)'!#REF!</definedName>
-    <definedName name="TransDist" localSheetId="0">#REF!</definedName>
+    <definedName name="TK_4601">'[10]REPORTE hoja2 (12h)'!#REF!</definedName>
     <definedName name="TransDist">#REF!</definedName>
-    <definedName name="TTKERO" localSheetId="0">#REF!</definedName>
     <definedName name="TTKERO">#REF!</definedName>
-    <definedName name="TTPI" localSheetId="0">#REF!</definedName>
     <definedName name="TTPI">#REF!</definedName>
-    <definedName name="TTRC" localSheetId="0">#REF!</definedName>
     <definedName name="TTRC">#REF!</definedName>
-    <definedName name="VAR" localSheetId="0">#REF!</definedName>
     <definedName name="VAR">#REF!</definedName>
-    <definedName name="VENTAS" localSheetId="0">#REF!</definedName>
     <definedName name="VENTAS">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -321,201 +215,13 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Estadistica</author>
-  </authors>
-  <commentList>
-    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{2E8027A5-087B-44E6-92DA-6A73DD51E527}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Estadistica:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Colocar Excedente de Suministrador de CNPC</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="124">
-  <si>
-    <t>REGISTRO DE VOLUMENES Y CALIDAD DEL GAS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
   <si>
     <t>FECHA:</t>
   </si>
   <si>
-    <t>I. VOLUMEN Y COMPOSICION DE GNA DE ENTRADA A PLANTA PARIÑAS</t>
-  </si>
-  <si>
-    <t>CORRIENTE</t>
-  </si>
-  <si>
-    <t>MEDIDOR</t>
-  </si>
-  <si>
-    <t>VOLUMEN FISCALIZADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIQUEZA </t>
-  </si>
-  <si>
-    <t>COMPOSICION (% MOLAR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (MPCS)</t>
-  </si>
-  <si>
-    <t>(GAL/MPCS)</t>
-  </si>
-  <si>
-    <t>C6+</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>iC4</t>
-  </si>
-  <si>
-    <t>nC4</t>
-  </si>
-  <si>
-    <t>neo C5</t>
-  </si>
-  <si>
-    <t>iC5</t>
-  </si>
-  <si>
-    <t>nC5</t>
-  </si>
-  <si>
-    <t>N2</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>CO2</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>O2</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>GNA DE LOTE Z69</t>
-  </si>
-  <si>
-    <t>P. de F. GNA de LOTE Z69</t>
-  </si>
-  <si>
-    <t>GNA DE CNPC</t>
-  </si>
-  <si>
-    <t>P. de F. GNA de CNPC</t>
-  </si>
-  <si>
-    <t>GNA DE LOTE VI</t>
-  </si>
-  <si>
-    <t>P. de F. de GNA de LOTE VI</t>
-  </si>
-  <si>
-    <t>GNA DE  LOTE I</t>
-  </si>
-  <si>
-    <t>P. de F. de GNA de LOTE I</t>
-  </si>
-  <si>
-    <t>GNA DE  LOTE IV</t>
-  </si>
-  <si>
-    <t>P. de F. de GNA de LOTE IV</t>
-  </si>
-  <si>
-    <t>GNA DE CNPC ADICIONAL</t>
-  </si>
-  <si>
-    <t>P. de F. de GNA de CNPC</t>
-  </si>
-  <si>
-    <t>NOTA: son volumenes fiscalizados a las 06:00 am y cuentan con la conformidad de EEPSA-UNNA-PERUPETRO</t>
-  </si>
-  <si>
-    <t>II. VOLUMEN DE GNS Y GAS COMBUSTIBLE PRODUCIDO EN PLANTA PARIÑAS</t>
-  </si>
-  <si>
-    <t>PRODUCTO</t>
-  </si>
-  <si>
-    <t>VOLUMEN</t>
-  </si>
-  <si>
-    <t>GNS</t>
-  </si>
-  <si>
-    <t>GAS COMBUSITIBLE</t>
-  </si>
-  <si>
-    <t>III. VOLUMEN DE LGN PRODUCIDOS EN PLANTA PARIÑAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>PRODUCCIÓN DIARIA</t>
-  </si>
-  <si>
-    <t>(BLS)</t>
-  </si>
-  <si>
-    <t>GLP</t>
-  </si>
-  <si>
-    <t>C5+</t>
-  </si>
-  <si>
     <t>BOLETA DE DETERMINACION DE VOLUMEN DE GNS, GAS COMBUSTIBLE,</t>
-  </si>
-  <si>
-    <t>UNNA - CNPC</t>
-  </si>
-  <si>
-    <t>Versión / Fecha
-01 / 15-04-16</t>
-  </si>
-  <si>
-    <t>Preparado por: UNNA</t>
-  </si>
-  <si>
-    <t>Aprobado por: CNPC</t>
   </si>
   <si>
     <t>FECHA</t>
@@ -596,24 +302,6 @@
     <t>(Ei=DixGNS Total)</t>
   </si>
   <si>
-    <t>LOTE Z69</t>
-  </si>
-  <si>
-    <t>CNPC</t>
-  </si>
-  <si>
-    <t>LOTE VI</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LOTE I</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LOTE IV</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Cuadro N° 2. Asignación de Gas Combustible al GNA Adicional del Lote X</t>
   </si>
   <si>
@@ -641,9 +329,6 @@
   </si>
   <si>
     <t>(Ji=IixGC Total)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNPC ADICIONAL </t>
   </si>
   <si>
     <t>Cuadro N° 3. Asignación de LGN al GNA Adicional del Lote X</t>
@@ -696,12 +381,6 @@
     <t>(Oi=NixLGN Total)</t>
   </si>
   <si>
-    <t>LOTE I</t>
-  </si>
-  <si>
-    <t>LOTE IV</t>
-  </si>
-  <si>
     <t>Gravedad especifica (Kg/L) GLP :</t>
   </si>
   <si>
@@ -726,44 +405,96 @@
     <t>{{CgnBls}}</t>
   </si>
   <si>
-    <t>{{GnsMpc}}</t>
-  </si>
-  <si>
-    <t>{{GcMpc}}</t>
-  </si>
-  <si>
-    <t>{{VolumenTotalDeGns}}</t>
-  </si>
-  <si>
-    <t>{{FlareGnaPertecienteEnel}}</t>
-  </si>
-  <si>
-    <t>{{VolumenTotalDeGnsEnMs}}</t>
-  </si>
-  <si>
     <t>{{item.Item}}</t>
   </si>
   <si>
-    <t>{{item.Sumistrador}}</t>
+    <t xml:space="preserve">Versión / Fecha
+01 / 26-02-24 </t>
+  </si>
+  <si>
+    <t>{{PreparadoPör}}</t>
+  </si>
+  <si>
+    <t>{{AprobadoPor}}</t>
+  </si>
+  <si>
+    <t>{{Compania}}</t>
+  </si>
+  <si>
+    <t>{{CgMpc}}</t>
+  </si>
+  <si>
+    <t>{{CnsMpc}}</t>
+  </si>
+  <si>
+    <t>{{VolumenTotalGnsEnMs}}</t>
+  </si>
+  <si>
+    <t>{{VolumenTotalGns}}</t>
+  </si>
+  <si>
+    <t>{{FlareGna}}</t>
+  </si>
+  <si>
+    <t>{{item.Volumen}}</t>
+  </si>
+  <si>
+    <t>{{item.ConcentracionC1}}</t>
+  </si>
+  <si>
+    <t>{{item.VolumenC1}}</t>
+  </si>
+  <si>
+    <t>{{item.FactoresDistribucion}}</t>
+  </si>
+  <si>
+    <t>{{item.AsignacionGns}}</t>
+  </si>
+  <si>
+    <t>{{VolumenTotalGasCombustible}}</t>
+  </si>
+  <si>
+    <t>{{VolumenProduccionTotalGlp}}</t>
+  </si>
+  <si>
+    <t>{{VolumenProduccionTotalCgn}}</t>
+  </si>
+  <si>
+    <t>{{VolumenProduccionTotalLgn}}</t>
+  </si>
+  <si>
+    <t>{{item.Riqueza}}</t>
+  </si>
+  <si>
+    <t>{{item.Contenido}}</t>
+  </si>
+  <si>
+    <t>{{GravedadEspecifica}}</t>
+  </si>
+  <si>
+    <t>{{VolumenProduccionTotalGlpCnpc}}</t>
+  </si>
+  <si>
+    <t>{{VolumenProduccionTotalCgnCnpc}}</t>
+  </si>
+  <si>
+    <t>{{item.Suministrador}}</t>
+  </si>
+  <si>
+    <t>Flare del GNA perteciente a  ENEL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="165" formatCode="0.000000000000000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.0000_)"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
-    <numFmt numFmtId="169" formatCode="0.0000000000000000"/>
-    <numFmt numFmtId="170" formatCode="#,##0.0000_ ;\-#,##0.0000\ "/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
-    <numFmt numFmtId="173" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -793,45 +524,6 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -868,15 +560,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -889,14 +574,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -966,19 +645,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1082,512 +748,294 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="3" borderId="6" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="11" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="11" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="11" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="11" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2 3" xfId="1" xr:uid="{2FABBF25-F10A-412C-95E7-73071C44A1D8}"/>
     <cellStyle name="Normal 3 5" xfId="2" xr:uid="{4AE76E0A-56E8-4E6F-A50B-5F9CE737D116}"/>
     <cellStyle name="Normal 4 4" xfId="3" xr:uid="{3FB5A7E5-7AD4-4765-AC5B-A794803B1BD0}"/>
     <cellStyle name="Normal 5 4" xfId="4" xr:uid="{F2C5A207-0A4F-4C97-84C6-388F9B0485BA}"/>
     <cellStyle name="Normal 8 5" xfId="5" xr:uid="{889B13DC-CF2D-43FE-B169-0CCE611AA90D}"/>
+    <cellStyle name="Porcentaje" xfId="6" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1706,23 +1154,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="MOLLENDO DIARIO"/>
-      <sheetName val="#¡REF"/>
-      <sheetName val="MOLLENDO_DIARIO"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="Correción 4606B"/>
       <sheetName val="Correción 4605B"/>
       <sheetName val="4605B &amp; 4606B"/>
@@ -28923,97 +28354,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="..."/>
-      <sheetName val=".."/>
-      <sheetName val="."/>
-      <sheetName val="Datos"/>
-      <sheetName val="3_GNA"/>
-      <sheetName val="1b_Tks"/>
-      <sheetName val="3_Gas"/>
-      <sheetName val="2_Ventas"/>
-      <sheetName val="5_BOLETA TANQUES"/>
-      <sheetName val="1_tanques"/>
-      <sheetName val="2_Líquidos"/>
-      <sheetName val="Imprimir Boleta"/>
-      <sheetName val="Boleta ENEL"/>
-      <sheetName val="Boleta GMP-Lote I"/>
-      <sheetName val="Boleta GMP-Lote IV"/>
-      <sheetName val="Boleta CNPC"/>
-      <sheetName val="5_Diario"/>
-      <sheetName val="7_Mensaje"/>
-      <sheetName val="8_Fila resumen"/>
-      <sheetName val="Nuevos Datos"/>
-      <sheetName val="EXISTENCIAS"/>
-      <sheetName val="GLP EXISTENCIAS"/>
-      <sheetName val="GLP - OSINERG"/>
-      <sheetName val="REPORTE"/>
-      <sheetName val="Turbina ENEL"/>
-      <sheetName val="PROPIEDADES"/>
-      <sheetName val="1_INGRESAR COMPOSICION"/>
-      <sheetName val="2_Cantidad y Calidad"/>
-      <sheetName val="3_FACTOR"/>
-      <sheetName val="BOLETA"/>
-      <sheetName val="BOLETA GNS"/>
-      <sheetName val="GAS-ENE 20"/>
-      <sheetName val="LGN-ENE 20"/>
-      <sheetName val="P.C LGN"/>
-      <sheetName val="P.C HAS"/>
-      <sheetName val="P.C GLP"/>
-      <sheetName val="REPORTE OSINERGMIN"/>
-      <sheetName val="Cantidad&amp;Calidad_CNPC"/>
-      <sheetName val="Boleta_CNPC"/>
-      <sheetName val="DATOS CORREOS"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="COMPRAS DE GAS"/>
       <sheetName val="Hoja1"/>
       <sheetName val="Hoja2"/>
@@ -30365,6 +29705,23 @@
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="MOLLENDO DIARIO"/>
+      <sheetName val="#¡REF"/>
+      <sheetName val="MOLLENDO_DIARIO"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -30666,2658 +30023,801 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7387B469-26E6-49E5-94CB-9B18B5C4D3BF}">
-  <sheetPr codeName="Hoja39">
-    <tabColor theme="3" tint="0.39997558519241921"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:FV63"/>
-  <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A14" zoomScale="85" zoomScaleNormal="69" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="31" style="4" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="9" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="4" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="4" customWidth="1"/>
-    <col min="17" max="18" width="11.28515625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="2" style="4" customWidth="1"/>
-    <col min="20" max="20" width="4" style="4" customWidth="1"/>
-    <col min="21" max="16384" width="11.28515625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:178" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="3"/>
-    </row>
-    <row r="2" spans="1:178" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" s="7"/>
-    </row>
-    <row r="3" spans="1:178" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="S3" s="7"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="8"/>
-      <c r="AH3" s="8"/>
-      <c r="AI3" s="8"/>
-      <c r="AJ3" s="9"/>
-      <c r="AK3" s="8"/>
-      <c r="AL3" s="8"/>
-      <c r="AM3" s="9"/>
-      <c r="AN3" s="8"/>
-      <c r="AO3" s="8"/>
-      <c r="AP3" s="8"/>
-      <c r="AQ3" s="8"/>
-      <c r="AR3" s="8"/>
-      <c r="AS3" s="8"/>
-      <c r="AT3" s="9"/>
-      <c r="AU3" s="8"/>
-      <c r="AV3" s="8"/>
-      <c r="AW3" s="8"/>
-      <c r="AX3" s="8"/>
-      <c r="BE3" s="8"/>
-      <c r="BF3" s="9"/>
-      <c r="BG3" s="8"/>
-      <c r="BH3" s="8"/>
-      <c r="BI3" s="8"/>
-      <c r="BJ3" s="9"/>
-      <c r="BK3" s="8"/>
-      <c r="BL3" s="8"/>
-      <c r="BM3" s="9"/>
-      <c r="BN3" s="8"/>
-      <c r="BO3" s="8"/>
-      <c r="BP3" s="8"/>
-      <c r="BQ3" s="8"/>
-      <c r="BR3" s="8"/>
-      <c r="BS3" s="8"/>
-      <c r="BT3" s="9"/>
-      <c r="BU3" s="8"/>
-      <c r="BV3" s="8"/>
-      <c r="BW3" s="8"/>
-      <c r="BX3" s="8"/>
-      <c r="CE3" s="8"/>
-      <c r="CF3" s="9"/>
-      <c r="CG3" s="8"/>
-      <c r="CH3" s="8"/>
-      <c r="CI3" s="8"/>
-      <c r="CJ3" s="9"/>
-      <c r="CK3" s="8"/>
-      <c r="CL3" s="8"/>
-      <c r="CM3" s="9"/>
-      <c r="CN3" s="8"/>
-      <c r="CO3" s="8"/>
-      <c r="CP3" s="8"/>
-      <c r="CQ3" s="8"/>
-      <c r="CR3" s="8"/>
-      <c r="CS3" s="8"/>
-      <c r="CT3" s="9"/>
-      <c r="CU3" s="8"/>
-      <c r="CV3" s="8"/>
-      <c r="CW3" s="8"/>
-      <c r="CX3" s="8"/>
-      <c r="DE3" s="8"/>
-      <c r="DF3" s="9"/>
-      <c r="DG3" s="8"/>
-      <c r="DH3" s="8"/>
-      <c r="DI3" s="8"/>
-      <c r="DJ3" s="9"/>
-      <c r="DK3" s="8"/>
-      <c r="DL3" s="8"/>
-      <c r="DM3" s="9"/>
-      <c r="DN3" s="8"/>
-      <c r="DO3" s="8"/>
-      <c r="DP3" s="8"/>
-      <c r="DQ3" s="8"/>
-      <c r="DR3" s="8"/>
-      <c r="DS3" s="8"/>
-      <c r="DT3" s="9"/>
-      <c r="DU3" s="8"/>
-      <c r="DV3" s="8"/>
-      <c r="DW3" s="8"/>
-      <c r="DX3" s="8"/>
-      <c r="EE3" s="8"/>
-      <c r="EF3" s="9"/>
-      <c r="EG3" s="8"/>
-      <c r="EH3" s="8"/>
-      <c r="EI3" s="8"/>
-      <c r="EJ3" s="9"/>
-      <c r="EK3" s="8"/>
-      <c r="EL3" s="8"/>
-      <c r="EM3" s="9"/>
-      <c r="EN3" s="8"/>
-      <c r="EO3" s="8"/>
-      <c r="EP3" s="8"/>
-      <c r="EQ3" s="8"/>
-      <c r="ER3" s="8"/>
-      <c r="ES3" s="8"/>
-      <c r="ET3" s="9"/>
-      <c r="EU3" s="8"/>
-      <c r="EV3" s="8"/>
-      <c r="EW3" s="8"/>
-      <c r="EX3" s="8"/>
-      <c r="FE3" s="8"/>
-      <c r="FF3" s="9"/>
-      <c r="FG3" s="8"/>
-      <c r="FH3" s="8"/>
-      <c r="FI3" s="8"/>
-      <c r="FJ3" s="9"/>
-      <c r="FK3" s="8"/>
-      <c r="FL3" s="8"/>
-      <c r="FM3" s="9"/>
-      <c r="FN3" s="8"/>
-      <c r="FO3" s="8"/>
-      <c r="FP3" s="8"/>
-      <c r="FQ3" s="8"/>
-      <c r="FR3" s="8"/>
-      <c r="FS3" s="8"/>
-      <c r="FT3" s="9"/>
-      <c r="FU3" s="8"/>
-      <c r="FV3" s="8"/>
-    </row>
-    <row r="4" spans="1:178" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="S4" s="7"/>
-    </row>
-    <row r="5" spans="1:178" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="13">
-        <v>45335</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="8"/>
-      <c r="S5" s="7"/>
-    </row>
-    <row r="6" spans="1:178" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="8"/>
-      <c r="S6" s="7"/>
-    </row>
-    <row r="7" spans="1:178" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="M7" s="18"/>
-      <c r="S7" s="7"/>
-    </row>
-    <row r="8" spans="1:178" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
-      <c r="S8" s="7"/>
-    </row>
-    <row r="9" spans="1:178" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="7"/>
-    </row>
-    <row r="10" spans="1:178" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="147" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="147" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="7"/>
-    </row>
-    <row r="11" spans="1:178" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="148"/>
-      <c r="C11" s="148"/>
-      <c r="D11" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="L11" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="N11" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="O11" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="P11" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q11" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="R11" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="S11" s="7"/>
-    </row>
-    <row r="12" spans="1:178" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="35">
-        <v>5408</v>
-      </c>
-      <c r="E12" s="36">
-        <v>1.2473000000000001</v>
-      </c>
-      <c r="F12" s="37">
-        <v>0.43445</v>
-      </c>
-      <c r="G12" s="37">
-        <v>1.4468700000000001</v>
-      </c>
-      <c r="H12" s="37">
-        <v>0.47659000000000001</v>
-      </c>
-      <c r="I12" s="37">
-        <v>0.73319999999999996</v>
-      </c>
-      <c r="J12" s="37">
-        <v>0</v>
-      </c>
-      <c r="K12" s="37">
-        <v>0.35255999999999998</v>
-      </c>
-      <c r="L12" s="37">
-        <v>0.21895000000000001</v>
-      </c>
-      <c r="M12" s="37">
-        <v>0.19077</v>
-      </c>
-      <c r="N12" s="37">
-        <v>88.622399999999999</v>
-      </c>
-      <c r="O12" s="37">
-        <v>1.2985500000000001</v>
-      </c>
-      <c r="P12" s="37">
-        <v>6.2256299999999998</v>
-      </c>
-      <c r="Q12" s="37">
-        <v>0</v>
-      </c>
-      <c r="R12" s="38">
-        <v>99.999970000000005</v>
-      </c>
-      <c r="S12" s="7"/>
-    </row>
-    <row r="13" spans="1:178" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="35">
-        <v>11000</v>
-      </c>
-      <c r="E13" s="36">
-        <v>1.5515000000000001</v>
-      </c>
-      <c r="F13" s="37">
-        <v>0.50429999999999997</v>
-      </c>
-      <c r="G13" s="37">
-        <v>1.6028</v>
-      </c>
-      <c r="H13" s="37">
-        <v>0.62380000000000002</v>
-      </c>
-      <c r="I13" s="37">
-        <v>0.7601</v>
-      </c>
-      <c r="J13" s="37">
-        <v>0</v>
-      </c>
-      <c r="K13" s="37">
-        <v>0.40179999999999999</v>
-      </c>
-      <c r="L13" s="37">
-        <v>0.22800000000000001</v>
-      </c>
-      <c r="M13" s="37">
-        <v>0.13650000000000001</v>
-      </c>
-      <c r="N13" s="37">
-        <v>91.364500000000007</v>
-      </c>
-      <c r="O13" s="37">
-        <v>0.65990000000000004</v>
-      </c>
-      <c r="P13" s="37">
-        <v>3.7183000000000002</v>
-      </c>
-      <c r="Q13" s="37">
-        <v>0</v>
-      </c>
-      <c r="R13" s="38">
-        <v>100</v>
-      </c>
-      <c r="S13" s="7"/>
-    </row>
-    <row r="14" spans="1:178" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="35">
-        <v>2794</v>
-      </c>
-      <c r="E14" s="36">
-        <v>2.5043000000000002</v>
-      </c>
-      <c r="F14" s="37">
-        <v>0.4572</v>
-      </c>
-      <c r="G14" s="37">
-        <v>3.4712999999999998</v>
-      </c>
-      <c r="H14" s="37">
-        <v>1.4480999999999999</v>
-      </c>
-      <c r="I14" s="37">
-        <v>1.9826999999999999</v>
-      </c>
-      <c r="J14" s="37">
-        <v>0</v>
-      </c>
-      <c r="K14" s="37">
-        <v>0.60780000000000001</v>
-      </c>
-      <c r="L14" s="37">
-        <v>0.6371</v>
-      </c>
-      <c r="M14" s="37">
-        <v>0.28760000000000002</v>
-      </c>
-      <c r="N14" s="37">
-        <v>84.820599999999999</v>
-      </c>
-      <c r="O14" s="37">
-        <v>0.30480000000000002</v>
-      </c>
-      <c r="P14" s="37">
-        <v>5.9828000000000001</v>
-      </c>
-      <c r="Q14" s="37">
-        <v>0</v>
-      </c>
-      <c r="R14" s="38">
-        <v>100</v>
-      </c>
-      <c r="S14" s="7"/>
-    </row>
-    <row r="15" spans="1:178" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="35">
-        <v>2767</v>
-      </c>
-      <c r="E15" s="36">
-        <v>2.2797999999999998</v>
-      </c>
-      <c r="F15" s="37">
-        <v>0.53932999999999998</v>
-      </c>
-      <c r="G15" s="37">
-        <v>3.2817699999999999</v>
-      </c>
-      <c r="H15" s="37">
-        <v>0.92988000000000004</v>
-      </c>
-      <c r="I15" s="37">
-        <v>1.33395</v>
-      </c>
-      <c r="J15" s="37">
-        <v>0</v>
-      </c>
-      <c r="K15" s="37">
-        <v>0.54295000000000004</v>
-      </c>
-      <c r="L15" s="37">
-        <v>0.33638000000000001</v>
-      </c>
-      <c r="M15" s="37">
-        <v>0.25928000000000001</v>
-      </c>
-      <c r="N15" s="37">
-        <v>85.917100000000005</v>
-      </c>
-      <c r="O15" s="37">
-        <v>0.36410999999999999</v>
-      </c>
-      <c r="P15" s="37">
-        <v>6.4952699999999997</v>
-      </c>
-      <c r="Q15" s="37">
-        <v>0</v>
-      </c>
-      <c r="R15" s="38">
-        <v>100.00002000000001</v>
-      </c>
-      <c r="S15" s="7"/>
-    </row>
-    <row r="16" spans="1:178" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="35">
-        <v>3113</v>
-      </c>
-      <c r="E16" s="36">
-        <v>1.9470000000000001</v>
-      </c>
-      <c r="F16" s="37">
-        <v>0.92011200000000004</v>
-      </c>
-      <c r="G16" s="37">
-        <v>3.0514199999999998</v>
-      </c>
-      <c r="H16" s="37">
-        <v>1.1364799999999999</v>
-      </c>
-      <c r="I16" s="37">
-        <v>1.4494499999999999</v>
-      </c>
-      <c r="J16" s="37">
-        <v>1.3789300000000001E-2</v>
-      </c>
-      <c r="K16" s="37">
-        <v>0.75622699999999998</v>
-      </c>
-      <c r="L16" s="37">
-        <v>0.364373</v>
-      </c>
-      <c r="M16" s="37">
-        <v>7.6122499999999996E-2</v>
-      </c>
-      <c r="N16" s="37">
-        <v>86.592200000000005</v>
-      </c>
-      <c r="O16" s="37">
-        <v>0.43686999999999998</v>
-      </c>
-      <c r="P16" s="37">
-        <v>5.2030000000000003</v>
-      </c>
-      <c r="Q16" s="37">
-        <v>0</v>
-      </c>
-      <c r="R16" s="38">
-        <v>100.0000438</v>
-      </c>
-      <c r="S16" s="7"/>
-    </row>
-    <row r="17" spans="1:19" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="40">
-        <v>789</v>
-      </c>
-      <c r="E17" s="41">
-        <v>1.5515000000000001</v>
-      </c>
-      <c r="F17" s="41">
-        <v>0.50429999999999997</v>
-      </c>
-      <c r="G17" s="41">
-        <v>1.6028</v>
-      </c>
-      <c r="H17" s="41">
-        <v>0.62380000000000002</v>
-      </c>
-      <c r="I17" s="41">
-        <v>0.7601</v>
-      </c>
-      <c r="J17" s="41">
-        <v>0</v>
-      </c>
-      <c r="K17" s="41">
-        <v>0.40179999999999999</v>
-      </c>
-      <c r="L17" s="41">
-        <v>0.22800000000000001</v>
-      </c>
-      <c r="M17" s="41">
-        <v>0.13650000000000001</v>
-      </c>
-      <c r="N17" s="41">
-        <v>91.364500000000007</v>
-      </c>
-      <c r="O17" s="41">
-        <v>0.65990000000000004</v>
-      </c>
-      <c r="P17" s="41">
-        <v>3.7183000000000002</v>
-      </c>
-      <c r="Q17" s="41">
-        <v>0</v>
-      </c>
-      <c r="R17" s="38">
-        <v>100</v>
-      </c>
-      <c r="S17" s="7"/>
-    </row>
-    <row r="18" spans="1:19" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="46"/>
-      <c r="R18" s="46"/>
-      <c r="S18" s="7"/>
-    </row>
-    <row r="19" spans="1:19" s="39" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="48"/>
-      <c r="O19" s="49"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="7"/>
-    </row>
-    <row r="20" spans="1:19" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="39"/>
-      <c r="S20" s="7"/>
-    </row>
-    <row r="21" spans="1:19" s="39" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="7"/>
-    </row>
-    <row r="22" spans="1:19" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="147" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="52"/>
-      <c r="O22" s="52"/>
-      <c r="P22" s="52"/>
-      <c r="Q22" s="52"/>
-      <c r="R22" s="43"/>
-      <c r="S22" s="7"/>
-    </row>
-    <row r="23" spans="1:19" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
-      <c r="B23" s="148"/>
-      <c r="C23" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="56"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="43"/>
-      <c r="S23" s="7"/>
-    </row>
-    <row r="24" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="58">
-        <v>9755.35</v>
-      </c>
-      <c r="D24" s="47"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="43"/>
-      <c r="R24" s="43"/>
-      <c r="S24" s="7"/>
-    </row>
-    <row r="25" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="58">
-        <v>1050.9000000000001</v>
-      </c>
-      <c r="D25" s="60"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="43"/>
-      <c r="R25" s="43"/>
-      <c r="S25" s="7"/>
-    </row>
-    <row r="26" spans="1:19" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="63"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="61"/>
-      <c r="N26" s="65"/>
-      <c r="O26" s="61"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="61"/>
-      <c r="R26" s="61"/>
-      <c r="S26" s="66"/>
-    </row>
-    <row r="27" spans="1:19" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="67"/>
-      <c r="B27" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G27" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="H27" s="4"/>
-      <c r="I27" s="64"/>
-      <c r="P27" s="4"/>
-      <c r="S27" s="66"/>
-    </row>
-    <row r="28" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="I28" s="14"/>
-      <c r="S28" s="7"/>
-    </row>
-    <row r="29" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="147" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="I29" s="14"/>
-      <c r="S29" s="7"/>
-    </row>
-    <row r="30" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="148"/>
-      <c r="C30" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="68"/>
-      <c r="S30" s="7"/>
-    </row>
-    <row r="31" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="69">
-        <v>685.64</v>
-      </c>
-      <c r="D31" s="70"/>
-      <c r="E31" s="71"/>
-      <c r="F31" s="71"/>
-      <c r="S31" s="7"/>
-    </row>
-    <row r="32" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="69">
-        <v>261.97000000000003</v>
-      </c>
-      <c r="D32" s="47"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="71"/>
-      <c r="S32" s="7"/>
-    </row>
-    <row r="33" spans="1:19" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="72"/>
-      <c r="S33" s="7"/>
-    </row>
-    <row r="34" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="73"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="76"/>
-      <c r="N34" s="43"/>
-      <c r="S34" s="7"/>
-    </row>
-    <row r="35" spans="1:19" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="77"/>
-      <c r="B35" s="78"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="78"/>
-      <c r="I35" s="78"/>
-      <c r="J35" s="78"/>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="78"/>
-      <c r="N35" s="78"/>
-      <c r="O35" s="78"/>
-      <c r="P35" s="78"/>
-      <c r="Q35" s="78"/>
-      <c r="R35" s="78"/>
-      <c r="S35" s="80"/>
-    </row>
-    <row r="36" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K36" s="76"/>
-      <c r="L36" s="76"/>
-      <c r="O36" s="74"/>
-    </row>
-    <row r="37" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O37" s="74"/>
-    </row>
-    <row r="38" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K38" s="76"/>
-      <c r="L38" s="76"/>
-      <c r="O38" s="74"/>
-    </row>
-    <row r="39" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K39" s="76"/>
-      <c r="L39" s="76"/>
-      <c r="O39" s="81"/>
-    </row>
-    <row r="40" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K40" s="76"/>
-      <c r="L40" s="76"/>
-    </row>
-    <row r="41" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="43"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="74"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="74"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="76"/>
-      <c r="L41" s="76"/>
-    </row>
-    <row r="43" spans="1:19" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="82"/>
-      <c r="B45" s="82"/>
-      <c r="C45" s="82"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="82"/>
-      <c r="F45" s="82"/>
-      <c r="G45" s="82"/>
-      <c r="H45" s="82"/>
-      <c r="I45" s="82"/>
-      <c r="J45" s="82"/>
-      <c r="K45" s="82"/>
-      <c r="L45" s="82"/>
-    </row>
-    <row r="46" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="82"/>
-      <c r="B46" s="82"/>
-      <c r="C46" s="82"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="82"/>
-      <c r="H46" s="82"/>
-      <c r="I46" s="82"/>
-      <c r="J46" s="82"/>
-      <c r="K46" s="82"/>
-      <c r="L46" s="82"/>
-    </row>
-    <row r="47" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="82"/>
-      <c r="B47" s="82"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="82"/>
-      <c r="F47" s="82"/>
-      <c r="G47" s="82"/>
-      <c r="H47" s="82"/>
-      <c r="I47" s="82"/>
-      <c r="J47" s="82"/>
-      <c r="K47" s="82"/>
-      <c r="L47" s="82"/>
-    </row>
-    <row r="48" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:178" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="82"/>
-      <c r="B49" s="82"/>
-      <c r="C49" s="82"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="82"/>
-      <c r="G49" s="82"/>
-      <c r="H49" s="82"/>
-      <c r="I49" s="82"/>
-      <c r="J49" s="82"/>
-      <c r="K49" s="82"/>
-      <c r="L49" s="82"/>
-    </row>
-    <row r="53" spans="1:178" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:178" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="82"/>
-      <c r="B54" s="82"/>
-      <c r="C54" s="82"/>
-      <c r="D54" s="82"/>
-      <c r="E54" s="82"/>
-      <c r="F54" s="82"/>
-      <c r="G54" s="82"/>
-      <c r="H54" s="82"/>
-      <c r="I54" s="82"/>
-      <c r="J54" s="82"/>
-      <c r="K54" s="82"/>
-      <c r="L54" s="82"/>
-    </row>
-    <row r="55" spans="1:178" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="82"/>
-      <c r="B55" s="82"/>
-      <c r="C55" s="82"/>
-      <c r="D55" s="82"/>
-      <c r="E55" s="82"/>
-      <c r="F55" s="82"/>
-      <c r="G55" s="82"/>
-      <c r="H55" s="82"/>
-      <c r="I55" s="82"/>
-      <c r="J55" s="82"/>
-      <c r="K55" s="82"/>
-      <c r="L55" s="82"/>
-    </row>
-    <row r="56" spans="1:178" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="82"/>
-      <c r="B56" s="82"/>
-      <c r="C56" s="82"/>
-      <c r="D56" s="82"/>
-      <c r="E56" s="82"/>
-      <c r="F56" s="82"/>
-      <c r="G56" s="82"/>
-      <c r="H56" s="82"/>
-      <c r="I56" s="82"/>
-      <c r="J56" s="82"/>
-      <c r="K56" s="82"/>
-      <c r="L56" s="82"/>
-    </row>
-    <row r="57" spans="1:178" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="82"/>
-      <c r="B57" s="82"/>
-      <c r="C57" s="82"/>
-      <c r="D57" s="82"/>
-      <c r="E57" s="82"/>
-      <c r="F57" s="82"/>
-      <c r="G57" s="82"/>
-      <c r="H57" s="82"/>
-      <c r="I57" s="82"/>
-      <c r="J57" s="82"/>
-      <c r="K57" s="82"/>
-      <c r="L57" s="82"/>
-    </row>
-    <row r="58" spans="1:178" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="82"/>
-      <c r="B58" s="82"/>
-      <c r="C58" s="82"/>
-      <c r="D58" s="82"/>
-      <c r="E58" s="82"/>
-      <c r="F58" s="82"/>
-      <c r="G58" s="82"/>
-      <c r="H58" s="82"/>
-      <c r="I58" s="82"/>
-      <c r="J58" s="82"/>
-      <c r="K58" s="82"/>
-      <c r="L58" s="82"/>
-      <c r="N58" s="146"/>
-      <c r="O58" s="146"/>
-      <c r="P58" s="146"/>
-      <c r="Q58" s="146"/>
-      <c r="R58" s="146"/>
-      <c r="S58" s="146"/>
-      <c r="T58" s="146"/>
-      <c r="U58" s="146"/>
-      <c r="V58" s="146"/>
-      <c r="W58" s="146"/>
-      <c r="X58" s="146"/>
-      <c r="Y58" s="146"/>
-      <c r="Z58" s="146"/>
-      <c r="AA58" s="146"/>
-      <c r="AB58" s="146"/>
-      <c r="AC58" s="146"/>
-      <c r="AD58" s="146"/>
-      <c r="AE58" s="146"/>
-      <c r="AF58" s="146"/>
-      <c r="AG58" s="146"/>
-      <c r="AH58" s="146"/>
-      <c r="AI58" s="146"/>
-      <c r="AJ58" s="146"/>
-      <c r="AK58" s="146"/>
-      <c r="AL58" s="146"/>
-      <c r="AM58" s="146"/>
-      <c r="AN58" s="146"/>
-      <c r="AO58" s="146"/>
-      <c r="AP58" s="146"/>
-      <c r="AQ58" s="146"/>
-      <c r="AR58" s="146"/>
-      <c r="AS58" s="146"/>
-      <c r="AT58" s="146"/>
-      <c r="AU58" s="146"/>
-      <c r="AV58" s="146"/>
-      <c r="AW58" s="146"/>
-      <c r="AX58" s="146"/>
-      <c r="AY58" s="146"/>
-      <c r="AZ58" s="146"/>
-      <c r="BA58" s="146"/>
-      <c r="BB58" s="146"/>
-      <c r="BC58" s="146"/>
-      <c r="BD58" s="146"/>
-      <c r="BE58" s="146"/>
-      <c r="BF58" s="146"/>
-      <c r="BG58" s="146"/>
-      <c r="BH58" s="146"/>
-      <c r="BI58" s="146"/>
-      <c r="BJ58" s="146"/>
-      <c r="BK58" s="146"/>
-      <c r="BL58" s="146"/>
-      <c r="BM58" s="146"/>
-      <c r="BN58" s="146"/>
-      <c r="BO58" s="146"/>
-      <c r="BP58" s="146"/>
-      <c r="BQ58" s="146"/>
-      <c r="BR58" s="146"/>
-      <c r="BS58" s="146"/>
-      <c r="BT58" s="146"/>
-      <c r="BU58" s="146"/>
-      <c r="BV58" s="146"/>
-      <c r="BW58" s="146"/>
-      <c r="BX58" s="146"/>
-      <c r="BY58" s="146"/>
-      <c r="BZ58" s="146"/>
-      <c r="CA58" s="146"/>
-      <c r="CB58" s="146"/>
-      <c r="CC58" s="146"/>
-      <c r="CD58" s="146"/>
-      <c r="CE58" s="146"/>
-      <c r="CF58" s="146"/>
-      <c r="CG58" s="146"/>
-      <c r="CH58" s="146"/>
-      <c r="CI58" s="146"/>
-      <c r="CJ58" s="146"/>
-      <c r="CK58" s="146"/>
-      <c r="CL58" s="146"/>
-      <c r="CM58" s="146"/>
-      <c r="CN58" s="146"/>
-      <c r="CO58" s="146"/>
-      <c r="CP58" s="146"/>
-      <c r="CQ58" s="146"/>
-      <c r="CR58" s="146"/>
-      <c r="CS58" s="146"/>
-      <c r="CT58" s="146"/>
-      <c r="CU58" s="146"/>
-      <c r="CV58" s="146"/>
-      <c r="CW58" s="146"/>
-      <c r="CX58" s="146"/>
-      <c r="CY58" s="146"/>
-      <c r="CZ58" s="146"/>
-      <c r="DA58" s="146"/>
-      <c r="DB58" s="146"/>
-      <c r="DC58" s="146"/>
-      <c r="DD58" s="146"/>
-      <c r="DE58" s="146"/>
-      <c r="DF58" s="146"/>
-      <c r="DG58" s="146"/>
-      <c r="DH58" s="146"/>
-      <c r="DI58" s="146"/>
-      <c r="DJ58" s="146"/>
-      <c r="DK58" s="146"/>
-      <c r="DL58" s="146"/>
-      <c r="DM58" s="146"/>
-      <c r="DN58" s="146"/>
-      <c r="DO58" s="146"/>
-      <c r="DP58" s="146"/>
-      <c r="DQ58" s="146"/>
-      <c r="DR58" s="146"/>
-      <c r="DS58" s="146"/>
-      <c r="DT58" s="146"/>
-      <c r="DU58" s="146"/>
-      <c r="DV58" s="146"/>
-      <c r="DW58" s="146"/>
-      <c r="DX58" s="146"/>
-      <c r="DY58" s="146"/>
-      <c r="DZ58" s="146"/>
-      <c r="EA58" s="146"/>
-      <c r="EB58" s="146"/>
-      <c r="EC58" s="146"/>
-      <c r="ED58" s="146"/>
-      <c r="EE58" s="146"/>
-      <c r="EF58" s="146"/>
-      <c r="EG58" s="146"/>
-      <c r="EH58" s="146"/>
-      <c r="EI58" s="146"/>
-      <c r="EJ58" s="146"/>
-      <c r="EK58" s="146"/>
-      <c r="EL58" s="146"/>
-      <c r="EM58" s="146"/>
-      <c r="EN58" s="146"/>
-      <c r="EO58" s="146"/>
-      <c r="EP58" s="146"/>
-      <c r="EQ58" s="146"/>
-      <c r="ER58" s="146"/>
-      <c r="ES58" s="146"/>
-      <c r="ET58" s="146"/>
-      <c r="EU58" s="146"/>
-      <c r="EV58" s="146"/>
-      <c r="EW58" s="146"/>
-      <c r="EX58" s="146"/>
-      <c r="EY58" s="146"/>
-      <c r="EZ58" s="146"/>
-      <c r="FA58" s="146"/>
-      <c r="FB58" s="146"/>
-      <c r="FC58" s="146"/>
-      <c r="FD58" s="146"/>
-      <c r="FE58" s="146"/>
-      <c r="FF58" s="146"/>
-      <c r="FG58" s="146"/>
-      <c r="FH58" s="146"/>
-      <c r="FI58" s="146"/>
-      <c r="FJ58" s="146"/>
-      <c r="FK58" s="146"/>
-      <c r="FL58" s="146"/>
-      <c r="FM58" s="146"/>
-      <c r="FN58" s="146"/>
-      <c r="FO58" s="146"/>
-      <c r="FP58" s="146"/>
-      <c r="FQ58" s="146"/>
-      <c r="FR58" s="146"/>
-      <c r="FS58" s="146"/>
-      <c r="FT58" s="146"/>
-      <c r="FU58" s="146"/>
-      <c r="FV58" s="146"/>
-    </row>
-    <row r="59" spans="1:178" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="82"/>
-      <c r="B59" s="82"/>
-      <c r="C59" s="82"/>
-      <c r="D59" s="82"/>
-      <c r="E59" s="82"/>
-      <c r="F59" s="82"/>
-      <c r="G59" s="82"/>
-      <c r="H59" s="82"/>
-      <c r="I59" s="82"/>
-      <c r="J59" s="82"/>
-      <c r="K59" s="82"/>
-      <c r="L59" s="82"/>
-      <c r="N59" s="146"/>
-      <c r="O59" s="146"/>
-      <c r="P59" s="146"/>
-      <c r="Q59" s="146"/>
-      <c r="R59" s="146"/>
-      <c r="S59" s="146"/>
-      <c r="T59" s="146"/>
-      <c r="U59" s="146"/>
-      <c r="V59" s="146"/>
-      <c r="W59" s="146"/>
-      <c r="X59" s="146"/>
-      <c r="Y59" s="146"/>
-      <c r="Z59" s="146"/>
-      <c r="AA59" s="146"/>
-      <c r="AB59" s="146"/>
-      <c r="AC59" s="146"/>
-      <c r="AD59" s="146"/>
-      <c r="AE59" s="146"/>
-      <c r="AF59" s="146"/>
-      <c r="AG59" s="146"/>
-      <c r="AH59" s="146"/>
-      <c r="AI59" s="146"/>
-      <c r="AJ59" s="146"/>
-      <c r="AK59" s="146"/>
-      <c r="AL59" s="146"/>
-      <c r="AM59" s="146"/>
-      <c r="AN59" s="146"/>
-      <c r="AO59" s="146"/>
-      <c r="AP59" s="146"/>
-      <c r="AQ59" s="146"/>
-      <c r="AR59" s="146"/>
-      <c r="AS59" s="146"/>
-      <c r="AT59" s="146"/>
-      <c r="AU59" s="146"/>
-      <c r="AV59" s="146"/>
-      <c r="AW59" s="146"/>
-      <c r="AX59" s="146"/>
-      <c r="AY59" s="146"/>
-      <c r="AZ59" s="146"/>
-      <c r="BA59" s="146"/>
-      <c r="BB59" s="146"/>
-      <c r="BC59" s="146"/>
-      <c r="BD59" s="146"/>
-      <c r="BE59" s="146"/>
-      <c r="BF59" s="146"/>
-      <c r="BG59" s="146"/>
-      <c r="BH59" s="146"/>
-      <c r="BI59" s="146"/>
-      <c r="BJ59" s="146"/>
-      <c r="BK59" s="146"/>
-      <c r="BL59" s="146"/>
-      <c r="BM59" s="146"/>
-      <c r="BN59" s="146"/>
-      <c r="BO59" s="146"/>
-      <c r="BP59" s="146"/>
-      <c r="BQ59" s="146"/>
-      <c r="BR59" s="146"/>
-      <c r="BS59" s="146"/>
-      <c r="BT59" s="146"/>
-      <c r="BU59" s="146"/>
-      <c r="BV59" s="146"/>
-      <c r="BW59" s="146"/>
-      <c r="BX59" s="146"/>
-      <c r="BY59" s="146"/>
-      <c r="BZ59" s="146"/>
-      <c r="CA59" s="146"/>
-      <c r="CB59" s="146"/>
-      <c r="CC59" s="146"/>
-      <c r="CD59" s="146"/>
-      <c r="CE59" s="146"/>
-      <c r="CF59" s="146"/>
-      <c r="CG59" s="146"/>
-      <c r="CH59" s="146"/>
-      <c r="CI59" s="146"/>
-      <c r="CJ59" s="146"/>
-      <c r="CK59" s="146"/>
-      <c r="CL59" s="146"/>
-      <c r="CM59" s="146"/>
-      <c r="CN59" s="146"/>
-      <c r="CO59" s="146"/>
-      <c r="CP59" s="146"/>
-      <c r="CQ59" s="146"/>
-      <c r="CR59" s="146"/>
-      <c r="CS59" s="146"/>
-      <c r="CT59" s="146"/>
-      <c r="CU59" s="146"/>
-      <c r="CV59" s="146"/>
-      <c r="CW59" s="146"/>
-      <c r="CX59" s="146"/>
-      <c r="CY59" s="146"/>
-      <c r="CZ59" s="146"/>
-      <c r="DA59" s="146"/>
-      <c r="DB59" s="146"/>
-      <c r="DC59" s="146"/>
-      <c r="DD59" s="146"/>
-      <c r="DE59" s="146"/>
-      <c r="DF59" s="146"/>
-      <c r="DG59" s="146"/>
-      <c r="DH59" s="146"/>
-      <c r="DI59" s="146"/>
-      <c r="DJ59" s="146"/>
-      <c r="DK59" s="146"/>
-      <c r="DL59" s="146"/>
-      <c r="DM59" s="146"/>
-      <c r="DN59" s="146"/>
-      <c r="DO59" s="146"/>
-      <c r="DP59" s="146"/>
-      <c r="DQ59" s="146"/>
-      <c r="DR59" s="146"/>
-      <c r="DS59" s="146"/>
-      <c r="DT59" s="146"/>
-      <c r="DU59" s="146"/>
-      <c r="DV59" s="146"/>
-      <c r="DW59" s="146"/>
-      <c r="DX59" s="146"/>
-      <c r="DY59" s="146"/>
-      <c r="DZ59" s="146"/>
-      <c r="EA59" s="146"/>
-      <c r="EB59" s="146"/>
-      <c r="EC59" s="146"/>
-      <c r="ED59" s="146"/>
-      <c r="EE59" s="146"/>
-      <c r="EF59" s="146"/>
-      <c r="EG59" s="146"/>
-      <c r="EH59" s="146"/>
-      <c r="EI59" s="146"/>
-      <c r="EJ59" s="146"/>
-      <c r="EK59" s="146"/>
-      <c r="EL59" s="146"/>
-      <c r="EM59" s="146"/>
-      <c r="EN59" s="146"/>
-      <c r="EO59" s="146"/>
-      <c r="EP59" s="146"/>
-      <c r="EQ59" s="146"/>
-      <c r="ER59" s="146"/>
-      <c r="ES59" s="146"/>
-      <c r="ET59" s="146"/>
-      <c r="EU59" s="146"/>
-      <c r="EV59" s="146"/>
-      <c r="EW59" s="146"/>
-      <c r="EX59" s="146"/>
-      <c r="EY59" s="146"/>
-      <c r="EZ59" s="146"/>
-      <c r="FA59" s="146"/>
-      <c r="FB59" s="146"/>
-      <c r="FC59" s="146"/>
-      <c r="FD59" s="146"/>
-      <c r="FE59" s="146"/>
-      <c r="FF59" s="146"/>
-      <c r="FG59" s="146"/>
-      <c r="FH59" s="146"/>
-      <c r="FI59" s="146"/>
-      <c r="FJ59" s="146"/>
-      <c r="FK59" s="146"/>
-      <c r="FL59" s="146"/>
-      <c r="FM59" s="146"/>
-      <c r="FN59" s="146"/>
-      <c r="FO59" s="146"/>
-      <c r="FP59" s="146"/>
-      <c r="FQ59" s="146"/>
-      <c r="FR59" s="146"/>
-      <c r="FS59" s="146"/>
-      <c r="FT59" s="146"/>
-      <c r="FU59" s="146"/>
-      <c r="FV59" s="146"/>
-    </row>
-    <row r="60" spans="1:178" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="149"/>
-      <c r="B60" s="149"/>
-      <c r="C60" s="149"/>
-      <c r="D60" s="149"/>
-      <c r="E60" s="61"/>
-      <c r="F60" s="150"/>
-      <c r="G60" s="150"/>
-      <c r="H60" s="150"/>
-      <c r="I60" s="150"/>
-      <c r="J60" s="150"/>
-      <c r="K60" s="150"/>
-      <c r="L60" s="150"/>
-      <c r="M60" s="150"/>
-    </row>
-    <row r="61" spans="1:178" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="9"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="20"/>
-      <c r="J61" s="83"/>
-      <c r="K61" s="83"/>
-      <c r="L61" s="83"/>
-      <c r="M61" s="9"/>
-    </row>
-    <row r="62" spans="1:178" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="9"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="J62" s="149"/>
-      <c r="K62" s="149"/>
-      <c r="L62" s="149"/>
-      <c r="M62" s="149"/>
-    </row>
-    <row r="63" spans="1:178" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J63" s="149"/>
-      <c r="K63" s="149"/>
-      <c r="L63" s="149"/>
-      <c r="M63" s="149"/>
-    </row>
-  </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="EI59:FF59"/>
-    <mergeCell ref="FG59:FV59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="F60:M60"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="CM59:DJ59"/>
-    <mergeCell ref="DK59:EH59"/>
-    <mergeCell ref="J63:M63"/>
-    <mergeCell ref="N59:T59"/>
-    <mergeCell ref="U59:AP59"/>
-    <mergeCell ref="AQ59:BN59"/>
-    <mergeCell ref="BO59:CL59"/>
-    <mergeCell ref="FG58:FV58"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="N58:T58"/>
-    <mergeCell ref="U58:AP58"/>
-    <mergeCell ref="AQ58:BN58"/>
-    <mergeCell ref="BO58:CL58"/>
-    <mergeCell ref="CM58:DJ58"/>
-    <mergeCell ref="DK58:EH58"/>
-    <mergeCell ref="EI58:FF58"/>
-  </mergeCells>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-  <colBreaks count="1" manualBreakCount="1">
-    <brk id="19" max="1048575" man="1"/>
-  </colBreaks>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA481EDA-EEBA-4371-ACC8-73E14ACDA808}">
   <sheetPr codeName="Hoja40">
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:U68"/>
+  <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47:E48"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35:I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4" style="92"/>
-    <col min="2" max="2" width="7.85546875" style="86" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="91" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" style="91" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="91" customWidth="1"/>
-    <col min="6" max="6" width="34" style="91" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" style="91" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" style="91" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" style="91" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="86" customWidth="1"/>
-    <col min="11" max="11" width="4" style="86"/>
-    <col min="12" max="12" width="8.28515625" style="86" bestFit="1" customWidth="1"/>
-    <col min="13" max="19" width="4" style="86"/>
-    <col min="20" max="20" width="31.5703125" style="86" customWidth="1"/>
-    <col min="21" max="21" width="12.28515625" style="86" customWidth="1"/>
-    <col min="22" max="16384" width="4" style="86"/>
+    <col min="1" max="1" width="4" style="10"/>
+    <col min="2" max="2" width="7.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="34" style="9" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="4" style="4"/>
+    <col min="12" max="12" width="8.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="19" width="4" style="4"/>
+    <col min="20" max="20" width="31.5703125" style="4" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" style="4" customWidth="1"/>
+    <col min="22" max="16384" width="4" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="151"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="157" t="s">
-        <v>48</v>
+      <c r="B1" s="73"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="79" t="s">
+        <v>1</v>
       </c>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
-      <c r="H1" s="158"/>
-      <c r="I1" s="85" t="s">
-        <v>49</v>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="3" t="s">
+        <v>61</v>
       </c>
-      <c r="J1" s="85"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="153"/>
-      <c r="C2" s="154"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="159"/>
-      <c r="F2" s="159"/>
-      <c r="G2" s="159"/>
-      <c r="H2" s="160"/>
-      <c r="I2" s="163" t="s">
-        <v>50</v>
+      <c r="B2" s="75"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="69" t="s">
+        <v>58</v>
       </c>
-      <c r="J2" s="163"/>
-      <c r="K2" s="88"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="155"/>
-      <c r="C3" s="156"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="90" t="s">
-        <v>51</v>
+      <c r="B3" s="77"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="8" t="s">
+        <v>59</v>
       </c>
-      <c r="J3" s="90" t="s">
-        <v>52</v>
+      <c r="J3" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="6"/>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="6"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="86" t="s">
-        <v>1</v>
+      <c r="B5" s="1"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="4" t="s">
+        <v>0</v>
       </c>
-      <c r="I5" s="94" t="s">
-        <v>113</v>
+      <c r="I5" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="6"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="95"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="6"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="96" t="s">
-        <v>53</v>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="14" t="s">
+        <v>2</v>
       </c>
-      <c r="E7" s="96" t="s">
-        <v>54</v>
+      <c r="E7" s="14" t="s">
+        <v>3</v>
       </c>
-      <c r="F7" s="96" t="s">
-        <v>55</v>
+      <c r="F7" s="14" t="s">
+        <v>4</v>
       </c>
-      <c r="G7" s="96" t="s">
-        <v>56</v>
+      <c r="G7" s="14" t="s">
+        <v>5</v>
       </c>
-      <c r="H7" s="96" t="s">
-        <v>57</v>
+      <c r="H7" s="14" t="s">
+        <v>6</v>
       </c>
-      <c r="I7" s="96" t="s">
-        <v>58</v>
+      <c r="I7" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="6"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="97" t="str">
+      <c r="B8" s="1"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="15" t="str">
         <f>+I5</f>
         <v>{{DiaOperativo}}</v>
       </c>
-      <c r="E8" s="98" t="s">
-        <v>114</v>
+      <c r="E8" s="16" t="s">
+        <v>54</v>
       </c>
-      <c r="F8" s="99" t="s">
-        <v>115</v>
+      <c r="F8" s="17" t="s">
+        <v>55</v>
       </c>
-      <c r="G8" s="99" t="s">
-        <v>116</v>
+      <c r="G8" s="17" t="s">
+        <v>56</v>
       </c>
-      <c r="H8" s="100" t="s">
-        <v>117</v>
+      <c r="H8" s="18" t="s">
+        <v>63</v>
       </c>
-      <c r="I8" s="100" t="s">
-        <v>118</v>
+      <c r="I8" s="18" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="6"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="95"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="93" t="s">
-        <v>59</v>
+      <c r="B10" s="1"/>
+      <c r="C10" s="11" t="s">
+        <v>8</v>
       </c>
-      <c r="D10" s="93"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="93"/>
-      <c r="G10" s="93"/>
-      <c r="H10" s="93"/>
-      <c r="I10" s="93"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
     </row>
     <row r="11" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="103"/>
+      <c r="B11" s="1"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="21"/>
     </row>
     <row r="12" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="104" t="s">
-        <v>60</v>
+      <c r="B12" s="1"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="22" t="s">
+        <v>9</v>
       </c>
-      <c r="E12" s="100" t="s">
-        <v>121</v>
+      <c r="E12" s="18" t="s">
+        <v>64</v>
       </c>
-      <c r="F12" s="86" t="s">
-        <v>61</v>
+      <c r="F12" s="4" t="s">
+        <v>10</v>
       </c>
-      <c r="G12" s="104" t="s">
-        <v>120</v>
+      <c r="G12" s="22" t="s">
+        <v>82</v>
       </c>
-      <c r="H12" s="100">
-        <f>'[6]Boleta ENEL'!E35</f>
-        <v>552</v>
+      <c r="H12" s="18" t="s">
+        <v>66</v>
       </c>
-      <c r="I12" s="86" t="s">
-        <v>61</v>
+      <c r="I12" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="6"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="106"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="106"/>
-      <c r="I13" s="86"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="6"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="104" t="s">
-        <v>62</v>
+      <c r="B14" s="1"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="22" t="s">
+        <v>11</v>
       </c>
-      <c r="E14" s="100" t="s">
-        <v>119</v>
+      <c r="E14" s="18" t="s">
+        <v>65</v>
       </c>
-      <c r="F14" s="86" t="s">
-        <v>61</v>
+      <c r="F14" s="4" t="s">
+        <v>10</v>
       </c>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="107"/>
+      <c r="C15" s="25"/>
     </row>
     <row r="16" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="164" t="s">
-        <v>63</v>
+      <c r="C16" s="61" t="s">
+        <v>12</v>
       </c>
-      <c r="D16" s="164" t="s">
-        <v>64</v>
+      <c r="D16" s="61" t="s">
+        <v>13</v>
       </c>
-      <c r="E16" s="165" t="s">
-        <v>65</v>
+      <c r="E16" s="62" t="s">
+        <v>14</v>
       </c>
-      <c r="F16" s="109" t="s">
-        <v>66</v>
+      <c r="F16" s="27" t="s">
+        <v>15</v>
       </c>
-      <c r="G16" s="109"/>
-      <c r="H16" s="109"/>
-      <c r="I16" s="110"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:21" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="6"/>
-      <c r="C17" s="164"/>
-      <c r="D17" s="164"/>
-      <c r="E17" s="166"/>
-      <c r="F17" s="111" t="s">
-        <v>67</v>
+      <c r="B17" s="1"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="29" t="s">
+        <v>16</v>
       </c>
-      <c r="G17" s="112" t="s">
-        <v>68</v>
+      <c r="G17" s="30" t="s">
+        <v>17</v>
       </c>
-      <c r="H17" s="112" t="s">
-        <v>69</v>
+      <c r="H17" s="30" t="s">
+        <v>18</v>
       </c>
-      <c r="I17" s="112" t="s">
-        <v>70</v>
+      <c r="I17" s="30" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B18" s="6"/>
-      <c r="C18" s="164"/>
-      <c r="D18" s="164"/>
-      <c r="E18" s="111" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+    </row>
+    <row r="19" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+      <c r="C19" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="104" t="s">
+      <c r="J19" s="36"/>
+    </row>
+    <row r="20" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="37"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="36"/>
+    </row>
+    <row r="21" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="40"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="36"/>
+    </row>
+    <row r="22" spans="1:21" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:21" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="1:21" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="68"/>
+      <c r="E24" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="G18" s="104" t="s">
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="28"/>
+    </row>
+    <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="65" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="66"/>
+    </row>
+    <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+      <c r="C30" s="61"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+    </row>
+    <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="66"/>
+    </row>
+    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="66"/>
+    </row>
+    <row r="33" spans="3:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="67"/>
+    </row>
+    <row r="34" spans="3:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="C35" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="I35" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="38"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="44"/>
+    </row>
+    <row r="38" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+    </row>
+    <row r="39" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="4"/>
+      <c r="D40" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="H18" s="104" t="s">
+      <c r="F40" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G40" s="45"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="4"/>
+      <c r="D41" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="I18" s="104" t="s">
+      <c r="F41" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G41" s="45"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="4"/>
+      <c r="D42" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="T18" s="105"/>
-      <c r="U18" s="105"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
     </row>
-    <row r="19" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="6"/>
-      <c r="C19" s="120" t="s">
-        <v>122</v>
+    <row r="43" spans="3:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="4"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="4" t="s">
+        <v>36</v>
       </c>
-      <c r="D19" s="114" t="s">
-        <v>123</v>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="45" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="61" t="s">
+        <v>12</v>
       </c>
-      <c r="E19" s="115"/>
-      <c r="F19" s="116"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="116"/>
-      <c r="I19" s="118"/>
-      <c r="J19" s="119"/>
+      <c r="D45" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="28"/>
     </row>
-    <row r="20" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="120"/>
-      <c r="D20" s="121"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="116"/>
-      <c r="G20" s="117"/>
-      <c r="H20" s="116"/>
-      <c r="I20" s="118"/>
-      <c r="J20" s="119"/>
+    <row r="46" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="H46" s="68" t="s">
+        <v>42</v>
+      </c>
+      <c r="I46" s="68" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="21" spans="1:21" s="125" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="92"/>
-      <c r="B21" s="86"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="114" t="s">
+    <row r="47" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="68"/>
+      <c r="G47" s="68"/>
+      <c r="H47" s="68"/>
+      <c r="I47" s="68"/>
+    </row>
+    <row r="48" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="61"/>
+      <c r="D48" s="61"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="68"/>
+      <c r="G48" s="68"/>
+      <c r="H48" s="68"/>
+      <c r="I48" s="68"/>
+    </row>
+    <row r="49" spans="3:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="68"/>
+      <c r="G49" s="68"/>
+      <c r="H49" s="68"/>
+      <c r="I49" s="68"/>
+    </row>
+    <row r="50" spans="3:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="61"/>
+      <c r="D50" s="61"/>
+      <c r="E50" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G50" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H50" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="I50" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="123">
-        <f>SUM(E19:E20)</f>
-        <v>0</v>
+      <c r="E51" s="43" t="s">
+        <v>67</v>
       </c>
-      <c r="F21" s="116" t="e">
-        <f>(E19*F19+E20*F20+#REF!*#REF!+#REF!*#REF!+#REF!*#REF!+#REF!*#REF!)/SUM(E19:E20)</f>
-        <v>#REF!</v>
+      <c r="F51" s="58" t="s">
+        <v>76</v>
       </c>
-      <c r="G21" s="123">
-        <f>SUM(G19:G20)</f>
-        <v>0</v>
+      <c r="G51" s="43" t="s">
+        <v>77</v>
       </c>
-      <c r="H21" s="116">
-        <f>SUM(H19:H20)</f>
-        <v>0</v>
+      <c r="H51" s="59" t="s">
+        <v>70</v>
       </c>
-      <c r="I21" s="124">
-        <f>SUM(I19:I20)</f>
-        <v>0</v>
+      <c r="I51" s="44" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:21" s="125" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="92"/>
-      <c r="B22" s="86"/>
-      <c r="C22" s="91"/>
-      <c r="D22" s="91"/>
-      <c r="E22" s="126"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="126"/>
-      <c r="H22" s="127"/>
-      <c r="I22" s="126"/>
+    <row r="52" spans="3:12" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C52" s="52"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
     </row>
-    <row r="23" spans="1:21" s="125" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="92"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="91"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="126"/>
-      <c r="G23" s="126"/>
-      <c r="H23" s="127"/>
-      <c r="I23" s="126"/>
+    <row r="53" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D53" s="60"/>
+      <c r="E53" s="60"/>
+      <c r="F53" s="60"/>
+      <c r="G53" s="60"/>
+      <c r="H53" s="60"/>
+      <c r="L53" s="46"/>
     </row>
-    <row r="24" spans="1:21" s="125" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="92"/>
-      <c r="B24" s="86"/>
-      <c r="C24" s="91"/>
-      <c r="E24" s="128"/>
-      <c r="F24" s="129"/>
-      <c r="G24" s="126"/>
-      <c r="H24" s="127"/>
-      <c r="I24" s="126"/>
+    <row r="54" spans="3:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D54" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="G54" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H54" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L54" s="46"/>
     </row>
-    <row r="25" spans="1:21" s="125" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="92"/>
-      <c r="B25" s="86"/>
-      <c r="C25" s="91"/>
-      <c r="D25" s="91"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="91"/>
-      <c r="I25" s="91"/>
-    </row>
-    <row r="26" spans="1:21" s="125" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="92"/>
-      <c r="B26" s="86"/>
-      <c r="C26" s="93" t="s">
-        <v>82</v>
+    <row r="55" spans="3:12" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G55" s="22" t="s">
+        <v>52</v>
       </c>
-      <c r="D26" s="93"/>
-      <c r="E26" s="93"/>
-      <c r="F26" s="93"/>
-      <c r="G26" s="93"/>
-      <c r="H26" s="93"/>
-      <c r="I26" s="93"/>
-    </row>
-    <row r="27" spans="1:21" s="125" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="92"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="91"/>
-      <c r="D27" s="102"/>
-      <c r="E27" s="102"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
-      <c r="H27" s="86"/>
-      <c r="I27" s="86"/>
-    </row>
-    <row r="28" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="86"/>
-      <c r="D28" s="104" t="s">
-        <v>83</v>
+      <c r="H55" s="17" t="s">
+        <v>80</v>
       </c>
-      <c r="E28" s="100">
-        <f>'Cantidad&amp;Calidad_CNPC'!C25</f>
-        <v>1050.9000000000001</v>
-      </c>
-      <c r="F28" s="86" t="s">
-        <v>61</v>
-      </c>
-      <c r="G28" s="86"/>
-      <c r="H28" s="86"/>
-      <c r="I28" s="86"/>
-    </row>
-    <row r="29" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="164" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="164" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="165" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" s="109" t="s">
-        <v>84</v>
-      </c>
-      <c r="G30" s="109"/>
-      <c r="H30" s="109"/>
-      <c r="I30" s="110"/>
-    </row>
-    <row r="31" spans="1:21" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="164"/>
-      <c r="D31" s="164"/>
-      <c r="E31" s="166"/>
-      <c r="F31" s="111" t="s">
-        <v>67</v>
-      </c>
-      <c r="G31" s="112" t="s">
-        <v>68</v>
-      </c>
-      <c r="H31" s="112" t="s">
-        <v>69</v>
-      </c>
-      <c r="I31" s="112" t="s">
-        <v>85</v>
+      <c r="I55" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.2">
-      <c r="C32" s="164"/>
-      <c r="D32" s="164"/>
-      <c r="E32" s="111" t="s">
-        <v>86</v>
-      </c>
-      <c r="F32" s="104" t="s">
-        <v>87</v>
-      </c>
-      <c r="G32" s="104" t="s">
-        <v>88</v>
-      </c>
-      <c r="H32" s="104" t="s">
-        <v>89</v>
-      </c>
-      <c r="I32" s="104" t="s">
-        <v>90</v>
-      </c>
+    <row r="56" spans="3:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G56" s="23"/>
+      <c r="H56" s="48"/>
     </row>
-    <row r="33" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="113">
-        <v>1</v>
-      </c>
-      <c r="D33" s="130" t="s">
-        <v>76</v>
-      </c>
-      <c r="E33" s="98">
-        <f>'Cantidad&amp;Calidad_CNPC'!D12</f>
-        <v>5408</v>
-      </c>
-      <c r="F33" s="131">
-        <f>('Cantidad&amp;Calidad_CNPC'!M12+'Cantidad&amp;Calidad_CNPC'!N12+'Cantidad&amp;Calidad_CNPC'!O12+'Cantidad&amp;Calidad_CNPC'!P12+'Cantidad&amp;Calidad_CNPC'!Q12)/100</f>
-        <v>0.96337349999999999</v>
-      </c>
-      <c r="G33" s="98">
-        <f t="shared" ref="G33:G38" si="0">E33*F33</f>
-        <v>5209.9238880000003</v>
-      </c>
-      <c r="H33" s="131">
-        <f t="shared" ref="H33:H38" si="1">G33/$G$39</f>
-        <v>0.21252352532360261</v>
-      </c>
-      <c r="I33" s="100">
-        <f>H33*$E$28</f>
-        <v>223.34097276257401</v>
-      </c>
+    <row r="57" spans="3:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G57" s="23"/>
+      <c r="H57" s="48"/>
     </row>
-    <row r="34" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="120">
-        <v>2</v>
-      </c>
-      <c r="D34" s="132" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" s="98">
-        <f>'Cantidad&amp;Calidad_CNPC'!D13</f>
-        <v>11000</v>
-      </c>
-      <c r="F34" s="131">
-        <f>('Cantidad&amp;Calidad_CNPC'!M13+'Cantidad&amp;Calidad_CNPC'!N13+'Cantidad&amp;Calidad_CNPC'!O13+'Cantidad&amp;Calidad_CNPC'!P13+'Cantidad&amp;Calidad_CNPC'!Q13)/100</f>
-        <v>0.95879199999999998</v>
-      </c>
-      <c r="G34" s="98">
-        <f t="shared" si="0"/>
-        <v>10546.712</v>
-      </c>
-      <c r="H34" s="131">
-        <f t="shared" si="1"/>
-        <v>0.43022210362331947</v>
-      </c>
-      <c r="I34" s="100">
-        <f t="shared" ref="I34:I37" si="2">H34*$E$28</f>
-        <v>452.12040869774648</v>
-      </c>
+    <row r="59" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E59" s="49"/>
+      <c r="G59" s="50"/>
     </row>
-    <row r="35" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="120">
-        <v>3</v>
-      </c>
-      <c r="D35" s="132" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="98">
-        <f>'Cantidad&amp;Calidad_CNPC'!D14</f>
-        <v>2794</v>
-      </c>
-      <c r="F35" s="131">
-        <f>('Cantidad&amp;Calidad_CNPC'!M14+'Cantidad&amp;Calidad_CNPC'!N14+'Cantidad&amp;Calidad_CNPC'!O14+'Cantidad&amp;Calidad_CNPC'!P14+'Cantidad&amp;Calidad_CNPC'!Q14)/100</f>
-        <v>0.91395799999999994</v>
-      </c>
-      <c r="G35" s="98">
-        <f t="shared" si="0"/>
-        <v>2553.5986519999997</v>
-      </c>
-      <c r="H35" s="131">
-        <f t="shared" si="1"/>
-        <v>0.10416654819749632</v>
-      </c>
-      <c r="I35" s="100">
-        <f t="shared" si="2"/>
-        <v>109.4686255007489</v>
-      </c>
+    <row r="60" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
     </row>
-    <row r="36" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="122">
-        <v>4</v>
-      </c>
-      <c r="D36" s="133" t="s">
-        <v>79</v>
-      </c>
-      <c r="E36" s="98">
-        <f>'Cantidad&amp;Calidad_CNPC'!D15</f>
-        <v>2767</v>
-      </c>
-      <c r="F36" s="131">
-        <f>('Cantidad&amp;Calidad_CNPC'!M15+'Cantidad&amp;Calidad_CNPC'!N15+'Cantidad&amp;Calidad_CNPC'!O15+'Cantidad&amp;Calidad_CNPC'!P15+'Cantidad&amp;Calidad_CNPC'!Q15)/100</f>
-        <v>0.93035760000000012</v>
-      </c>
-      <c r="G36" s="98">
-        <f t="shared" si="0"/>
-        <v>2574.2994792000004</v>
-      </c>
-      <c r="H36" s="131">
-        <f t="shared" si="1"/>
-        <v>0.10501097757271081</v>
-      </c>
-      <c r="I36" s="100">
-        <f t="shared" si="2"/>
-        <v>110.3560363311618</v>
-      </c>
+    <row r="61" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
     </row>
-    <row r="37" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="122">
-        <v>5</v>
-      </c>
-      <c r="D37" s="133" t="s">
-        <v>80</v>
-      </c>
-      <c r="E37" s="98">
-        <f>'Cantidad&amp;Calidad_CNPC'!D16</f>
-        <v>3113</v>
-      </c>
-      <c r="F37" s="131">
-        <f>('Cantidad&amp;Calidad_CNPC'!M16+'Cantidad&amp;Calidad_CNPC'!N16+'Cantidad&amp;Calidad_CNPC'!O16+'Cantidad&amp;Calidad_CNPC'!P16+'Cantidad&amp;Calidad_CNPC'!Q16)/100</f>
-        <v>0.92308192500000008</v>
-      </c>
-      <c r="G37" s="98">
-        <f t="shared" si="0"/>
-        <v>2873.5540325250004</v>
-      </c>
-      <c r="H37" s="131">
-        <f t="shared" si="1"/>
-        <v>0.11721818712297996</v>
-      </c>
-      <c r="I37" s="100">
-        <f t="shared" si="2"/>
-        <v>123.18459284753965</v>
-      </c>
-    </row>
-    <row r="38" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="120">
-        <v>6</v>
-      </c>
-      <c r="D38" s="132" t="s">
-        <v>91</v>
-      </c>
-      <c r="E38" s="98">
-        <f>'Cantidad&amp;Calidad_CNPC'!D17</f>
-        <v>789</v>
-      </c>
-      <c r="F38" s="131">
-        <f>('Cantidad&amp;Calidad_CNPC'!M17+'Cantidad&amp;Calidad_CNPC'!N17+'Cantidad&amp;Calidad_CNPC'!O17+'Cantidad&amp;Calidad_CNPC'!P17+'Cantidad&amp;Calidad_CNPC'!Q17)/100</f>
-        <v>0.95879199999999998</v>
-      </c>
-      <c r="G38" s="98">
-        <f t="shared" si="0"/>
-        <v>756.48688800000002</v>
-      </c>
-      <c r="H38" s="131">
-        <f t="shared" si="1"/>
-        <v>3.0858658159890827E-2</v>
-      </c>
-      <c r="I38" s="100">
-        <f>H38*$E$28</f>
-        <v>32.429363860229273</v>
-      </c>
-      <c r="J38" s="134"/>
-    </row>
-    <row r="39" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="121"/>
-      <c r="D39" s="130" t="s">
-        <v>81</v>
-      </c>
-      <c r="E39" s="135">
-        <f>SUM(E33:E38)</f>
-        <v>25871</v>
-      </c>
-      <c r="F39" s="131">
-        <f>(E33*F33+E34*F34+E35*F35+E36*F36+E37*F37+E38*F38)/SUM(E33:E38)</f>
-        <v>0.94756967027656447</v>
-      </c>
-      <c r="G39" s="135">
-        <f>SUM(G33:G38)</f>
-        <v>24514.574939725</v>
-      </c>
-      <c r="H39" s="131">
-        <f>SUM(H33:H38)</f>
-        <v>1</v>
-      </c>
-      <c r="I39" s="136">
-        <f>SUM(I33:I38)</f>
-        <v>1050.9000000000001</v>
-      </c>
-    </row>
-    <row r="41" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="93" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="93"/>
-      <c r="E41" s="93"/>
-      <c r="F41" s="93"/>
-      <c r="G41" s="93"/>
-      <c r="H41" s="93"/>
-      <c r="I41" s="93"/>
-    </row>
-    <row r="42" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D42" s="102"/>
-      <c r="E42" s="102"/>
-      <c r="F42" s="86"/>
-      <c r="G42" s="86"/>
-      <c r="H42" s="86"/>
-      <c r="I42" s="86"/>
-    </row>
-    <row r="43" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C43" s="86"/>
-      <c r="D43" s="104" t="s">
-        <v>93</v>
-      </c>
-      <c r="E43" s="100">
-        <f>'Cantidad&amp;Calidad_CNPC'!C31</f>
-        <v>685.64</v>
-      </c>
-      <c r="F43" s="86" t="s">
-        <v>94</v>
-      </c>
-      <c r="G43" s="137"/>
-      <c r="H43" s="86"/>
-      <c r="I43" s="86"/>
-    </row>
-    <row r="44" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C44" s="86"/>
-      <c r="D44" s="104" t="s">
-        <v>95</v>
-      </c>
-      <c r="E44" s="100">
-        <f>'Cantidad&amp;Calidad_CNPC'!C32</f>
-        <v>261.97000000000003</v>
-      </c>
-      <c r="F44" s="86" t="s">
-        <v>94</v>
-      </c>
-      <c r="G44" s="137"/>
-      <c r="H44" s="86"/>
-      <c r="I44" s="86"/>
-    </row>
-    <row r="45" spans="3:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="86"/>
-      <c r="D45" s="104" t="s">
-        <v>96</v>
-      </c>
-      <c r="E45" s="100">
-        <f>E43+E44</f>
-        <v>947.61</v>
-      </c>
-      <c r="F45" s="86" t="s">
-        <v>94</v>
-      </c>
-      <c r="G45" s="86"/>
-      <c r="H45" s="86"/>
-      <c r="I45" s="86"/>
-    </row>
-    <row r="47" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="164" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="164" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47" s="165" t="s">
-        <v>65</v>
-      </c>
-      <c r="F47" s="109" t="s">
-        <v>97</v>
-      </c>
-      <c r="G47" s="109"/>
-      <c r="H47" s="109"/>
-      <c r="I47" s="110"/>
-    </row>
-    <row r="48" spans="3:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C48" s="164"/>
-      <c r="D48" s="164"/>
-      <c r="E48" s="166"/>
-      <c r="F48" s="104" t="s">
-        <v>98</v>
-      </c>
-      <c r="G48" s="104" t="s">
-        <v>99</v>
-      </c>
-      <c r="H48" s="104" t="s">
-        <v>100</v>
-      </c>
-      <c r="I48" s="104" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="49" spans="3:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C49" s="164"/>
-      <c r="D49" s="164"/>
-      <c r="E49" s="111" t="s">
-        <v>102</v>
-      </c>
-      <c r="F49" s="104" t="s">
-        <v>103</v>
-      </c>
-      <c r="G49" s="104" t="s">
-        <v>104</v>
-      </c>
-      <c r="H49" s="104" t="s">
-        <v>105</v>
-      </c>
-      <c r="I49" s="104" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C50" s="138">
-        <v>1</v>
-      </c>
-      <c r="D50" s="130" t="s">
-        <v>76</v>
-      </c>
-      <c r="E50" s="98">
-        <f>'Cantidad&amp;Calidad_CNPC'!D12</f>
-        <v>5408</v>
-      </c>
-      <c r="F50" s="139">
-        <f>+'Cantidad&amp;Calidad_CNPC'!E12</f>
-        <v>1.2473000000000001</v>
-      </c>
-      <c r="G50" s="98">
-        <f t="shared" ref="G50:G53" si="3">E50*F50</f>
-        <v>6745.3984</v>
-      </c>
-      <c r="H50" s="131">
-        <f t="shared" ref="H50:H54" si="4">G50/$G$56</f>
-        <v>0.15191564208470748</v>
-      </c>
-      <c r="I50" s="100">
-        <f>ROUND(H50*$E$45,2)</f>
-        <v>143.96</v>
-      </c>
-    </row>
-    <row r="51" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="108">
-        <v>2</v>
-      </c>
-      <c r="D51" s="132" t="s">
-        <v>77</v>
-      </c>
-      <c r="E51" s="98">
-        <f>'Cantidad&amp;Calidad_CNPC'!D13</f>
-        <v>11000</v>
-      </c>
-      <c r="F51" s="139">
-        <f>+'Cantidad&amp;Calidad_CNPC'!E13</f>
-        <v>1.5515000000000001</v>
-      </c>
-      <c r="G51" s="98">
-        <f t="shared" si="3"/>
-        <v>17066.5</v>
-      </c>
-      <c r="H51" s="131">
-        <f t="shared" si="4"/>
-        <v>0.38436103427762847</v>
-      </c>
-      <c r="I51" s="100">
-        <f>ROUND(H51*$E$45,2)</f>
-        <v>364.22</v>
-      </c>
-    </row>
-    <row r="52" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C52" s="108">
-        <v>3</v>
-      </c>
-      <c r="D52" s="132" t="s">
-        <v>78</v>
-      </c>
-      <c r="E52" s="98">
-        <f>'Cantidad&amp;Calidad_CNPC'!D14</f>
-        <v>2794</v>
-      </c>
-      <c r="F52" s="139">
-        <f>+'Cantidad&amp;Calidad_CNPC'!E14</f>
-        <v>2.5043000000000002</v>
-      </c>
-      <c r="G52" s="98">
-        <f t="shared" si="3"/>
-        <v>6997.0142000000005</v>
-      </c>
-      <c r="H52" s="131">
-        <f t="shared" si="4"/>
-        <v>0.15758237569315639</v>
-      </c>
-      <c r="I52" s="100">
-        <f>ROUND(H52*$E$45,2)</f>
-        <v>149.33000000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C53" s="140">
-        <v>4</v>
-      </c>
-      <c r="D53" s="133" t="s">
-        <v>107</v>
-      </c>
-      <c r="E53" s="98">
-        <f>'Cantidad&amp;Calidad_CNPC'!D15</f>
-        <v>2767</v>
-      </c>
-      <c r="F53" s="139">
-        <f>+'Cantidad&amp;Calidad_CNPC'!E15</f>
-        <v>2.2797999999999998</v>
-      </c>
-      <c r="G53" s="98">
-        <f t="shared" si="3"/>
-        <v>6308.2065999999995</v>
-      </c>
-      <c r="H53" s="131">
-        <f t="shared" si="4"/>
-        <v>0.14206948192148139</v>
-      </c>
-      <c r="I53" s="100">
-        <f>ROUND(H53*$E$45,2)</f>
-        <v>134.63</v>
-      </c>
-    </row>
-    <row r="54" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C54" s="140">
-        <v>5</v>
-      </c>
-      <c r="D54" s="133" t="s">
-        <v>108</v>
-      </c>
-      <c r="E54" s="98">
-        <f>'Cantidad&amp;Calidad_CNPC'!D16</f>
-        <v>3113</v>
-      </c>
-      <c r="F54" s="139">
-        <f>+'Cantidad&amp;Calidad_CNPC'!E16</f>
-        <v>1.9470000000000001</v>
-      </c>
-      <c r="G54" s="98">
-        <f>E54*F54</f>
-        <v>6061.0110000000004</v>
-      </c>
-      <c r="H54" s="131">
-        <f t="shared" si="4"/>
-        <v>0.13650229729165814</v>
-      </c>
-      <c r="I54" s="100">
-        <f>ROUND(H54*$E$45,2)</f>
-        <v>129.35</v>
-      </c>
-    </row>
-    <row r="55" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C55" s="108">
-        <v>6</v>
-      </c>
-      <c r="D55" s="132" t="s">
-        <v>91</v>
-      </c>
-      <c r="E55" s="98">
-        <f>'Cantidad&amp;Calidad_CNPC'!D17</f>
-        <v>789</v>
-      </c>
-      <c r="F55" s="139">
-        <f>+'Cantidad&amp;Calidad_CNPC'!E17</f>
-        <v>1.5515000000000001</v>
-      </c>
-      <c r="G55" s="98">
-        <f>E55*F55</f>
-        <v>1224.1335000000001</v>
-      </c>
-      <c r="H55" s="131">
-        <f>G55/$G$56</f>
-        <v>2.7569168731368082E-2</v>
-      </c>
-      <c r="I55" s="100">
-        <f>ROUNDDOWN(H55*$E$45,2)</f>
-        <v>26.12</v>
-      </c>
-    </row>
-    <row r="56" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C56" s="121"/>
-      <c r="D56" s="130" t="s">
-        <v>81</v>
-      </c>
-      <c r="E56" s="135">
-        <f>SUM(E50:E55)</f>
-        <v>25871</v>
-      </c>
-      <c r="F56" s="139">
-        <f>(E50*F50+E51*F51+E52*F52+E53*F53+E55*F55)/SUM(E50:E55)</f>
-        <v>1.4820166479842296</v>
-      </c>
-      <c r="G56" s="135">
-        <f>SUM(G50:G55)</f>
-        <v>44402.263700000003</v>
-      </c>
-      <c r="H56" s="131">
-        <f>SUM(H50:H55)</f>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="I56" s="100">
-        <f>SUM(I50:I55)</f>
-        <v>947.61000000000013</v>
-      </c>
-      <c r="L56" s="141"/>
-    </row>
-    <row r="57" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D57" s="167"/>
-      <c r="E57" s="167"/>
-      <c r="F57" s="167"/>
-      <c r="G57" s="167"/>
-      <c r="H57" s="167"/>
-      <c r="L57" s="141"/>
-    </row>
-    <row r="58" spans="3:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D58" s="108" t="s">
-        <v>109</v>
-      </c>
-      <c r="E58" s="142">
-        <v>0.53590000000000004</v>
-      </c>
-      <c r="G58" s="104" t="s">
-        <v>110</v>
-      </c>
-      <c r="H58" s="99">
-        <f>I55*E43/E45</f>
-        <v>18.89903736769346</v>
-      </c>
-      <c r="I58" s="86" t="s">
-        <v>111</v>
-      </c>
-      <c r="L58" s="141"/>
-    </row>
-    <row r="59" spans="3:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G59" s="104" t="s">
-        <v>112</v>
-      </c>
-      <c r="H59" s="99">
-        <f>I55*(E44/E45)+0</f>
-        <v>7.2209626323065406</v>
-      </c>
-      <c r="I59" s="91" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="60" spans="3:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G60" s="105"/>
-      <c r="H60" s="143"/>
-    </row>
-    <row r="61" spans="3:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G61" s="105"/>
-      <c r="H61" s="143"/>
+    <row r="62" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
     </row>
     <row r="63" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E63" s="144"/>
-      <c r="G63" s="145"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
     </row>
     <row r="64" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G64" s="86"/>
-      <c r="H64" s="86"/>
-      <c r="I64" s="86"/>
-    </row>
-    <row r="65" spans="7:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G65" s="86"/>
-      <c r="H65" s="86"/>
-      <c r="I65" s="86"/>
-    </row>
-    <row r="66" spans="7:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G66" s="86"/>
-      <c r="H66" s="86"/>
-      <c r="I66" s="86"/>
-    </row>
-    <row r="67" spans="7:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G67" s="86"/>
-      <c r="H67" s="86"/>
-      <c r="I67" s="86"/>
-    </row>
-    <row r="68" spans="7:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G68" s="86"/>
-      <c r="H68" s="86"/>
-      <c r="I68" s="86"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="D57:H57"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="B1:C3"/>
-    <mergeCell ref="E1:H3"/>
+  <mergeCells count="25">
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="E16:E17"/>
+    <mergeCell ref="I46:I49"/>
+    <mergeCell ref="I28:I33"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="B1:C3"/>
+    <mergeCell ref="E1:H3"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D53:H53"/>
+    <mergeCell ref="C27:C34"/>
+    <mergeCell ref="D27:D34"/>
+    <mergeCell ref="C45:C50"/>
+    <mergeCell ref="D45:D50"/>
+    <mergeCell ref="E45:E49"/>
+    <mergeCell ref="E27:E33"/>
+    <mergeCell ref="F28:F33"/>
+    <mergeCell ref="G28:G33"/>
+    <mergeCell ref="H28:H33"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="G46:G49"/>
+    <mergeCell ref="H46:H49"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0.19685039370078741" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>